<commit_message>
lower circs in datasheet
</commit_message>
<xml_diff>
--- a/tests/generalized.xlsx
+++ b/tests/generalized.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="1485" windowWidth="19425" windowHeight="10965" tabRatio="901" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="2200" yWindow="1480" windowWidth="19420" windowHeight="10960" tabRatio="901" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,12 @@
     <sheet name="Partnerships &amp; transitions" sheetId="10" r:id="rId11"/>
     <sheet name="Constants" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -519,8 +524,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="7">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="#,##0_ ;\-#,##0\ "/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
@@ -744,12 +749,12 @@
   </borders>
   <cellStyleXfs count="306">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -812,7 +817,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1086,7 +1091,7 @@
     <xf numFmtId="166" fontId="0" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1845,34 +1850,34 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="89.28515625" customWidth="1"/>
+    <col min="1" max="1" width="89.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="75" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="76"/>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="76"/>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="25"/>
     </row>
-    <row r="5" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="28">
       <c r="A5" s="25" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="25"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="26" t="s">
         <v>97</v>
       </c>
@@ -1899,14 +1904,14 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25">
       <c r="C2" s="3">
         <v>2000</v>
       </c>
@@ -1974,7 +1979,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25">
       <c r="B3" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2007,7 +2012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25">
       <c r="B4" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2040,7 +2045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25">
       <c r="B5" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2073,7 +2078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25">
       <c r="B6" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -2106,7 +2111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25">
       <c r="B7" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -2139,7 +2144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25">
       <c r="B8" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -2172,7 +2177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25">
       <c r="B9" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -2205,7 +2210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" s="50" customFormat="1">
       <c r="B10" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -2238,7 +2243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" s="50" customFormat="1">
       <c r="B11" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -2271,12 +2276,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25">
       <c r="A15" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25">
       <c r="C16" s="3">
         <v>2000</v>
       </c>
@@ -2344,7 +2349,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25">
       <c r="B17" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2377,7 +2382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25">
       <c r="B18" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2410,7 +2415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25">
       <c r="B19" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2443,7 +2448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25">
       <c r="B20" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -2476,7 +2481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25">
       <c r="B21" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -2509,7 +2514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25">
       <c r="B22" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -2542,7 +2547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25">
       <c r="B23" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -2575,7 +2580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" s="50" customFormat="1">
       <c r="B24" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -2608,7 +2613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" s="50" customFormat="1">
       <c r="B25" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -2641,12 +2646,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25">
       <c r="A29" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25">
       <c r="C30" s="3">
         <v>2000</v>
       </c>
@@ -2714,7 +2719,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25">
       <c r="B31" s="3" t="s">
         <v>36</v>
       </c>
@@ -2765,18 +2770,18 @@
       <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="11" width="12.7109375" style="50" customWidth="1"/>
+    <col min="3" max="9" width="12.6640625" customWidth="1"/>
+    <col min="10" max="11" width="12.6640625" style="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="C2" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2814,7 +2819,7 @@
         <v>F 50+</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="B3" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2829,7 +2834,7 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="B4" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2850,7 +2855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="B5" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2867,7 +2872,7 @@
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="B6" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -2882,7 +2887,7 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="B7" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -2897,7 +2902,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="B8" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -2918,7 +2923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="B9" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -2933,7 +2938,7 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="50" customFormat="1">
       <c r="B10" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -2954,7 +2959,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="50" customFormat="1">
       <c r="B11" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -2969,12 +2974,12 @@
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="C16" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3012,7 +3017,7 @@
         <v>F 50+</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="B17" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3027,7 +3032,7 @@
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="B18" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3048,7 +3053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="B19" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3065,7 +3070,7 @@
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="B20" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -3080,7 +3085,7 @@
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="B21" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -3095,7 +3100,7 @@
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="B22" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -3116,7 +3121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="B23" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -3131,7 +3136,7 @@
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="50" customFormat="1">
       <c r="B24" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -3152,7 +3157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="50" customFormat="1">
       <c r="B25" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -3167,12 +3172,12 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="C30" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3210,7 +3215,7 @@
         <v>F 50+</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="B31" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3225,7 +3230,7 @@
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="B32" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3242,7 +3247,7 @@
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="B33" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3257,7 +3262,7 @@
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="B34" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -3272,7 +3277,7 @@
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="B35" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -3287,7 +3292,7 @@
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="B36" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -3302,7 +3307,7 @@
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="B37" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -3317,7 +3322,7 @@
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
     </row>
-    <row r="38" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" s="50" customFormat="1">
       <c r="B38" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -3332,7 +3337,7 @@
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
     </row>
-    <row r="39" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" s="50" customFormat="1">
       <c r="B39" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -3347,12 +3352,12 @@
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11">
       <c r="A43" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11">
       <c r="C44" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3390,7 +3395,7 @@
         <v>F 50+</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11">
       <c r="B45" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3405,7 +3410,7 @@
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11">
       <c r="B46" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3420,7 +3425,7 @@
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11">
       <c r="B47" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3435,7 +3440,7 @@
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11">
       <c r="B48" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -3450,7 +3455,7 @@
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11">
       <c r="B49" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -3465,7 +3470,7 @@
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11">
       <c r="B50" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -3480,7 +3485,7 @@
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11">
       <c r="B51" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -3495,7 +3500,7 @@
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
     </row>
-    <row r="52" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" s="50" customFormat="1">
       <c r="B52" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -3510,7 +3515,7 @@
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
     </row>
-    <row r="53" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" s="50" customFormat="1">
       <c r="B53" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -3525,12 +3530,12 @@
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
     </row>
-    <row r="57" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" s="50" customFormat="1">
       <c r="A57" s="51" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" s="50" customFormat="1">
       <c r="C58" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3568,7 +3573,7 @@
         <v>F 50+</v>
       </c>
     </row>
-    <row r="59" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" s="50" customFormat="1">
       <c r="B59" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3587,7 +3592,7 @@
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
     </row>
-    <row r="60" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" s="50" customFormat="1">
       <c r="B60" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -3602,7 +3607,7 @@
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
     </row>
-    <row r="61" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" s="50" customFormat="1">
       <c r="B61" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -3621,7 +3626,7 @@
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
     </row>
-    <row r="62" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" s="50" customFormat="1">
       <c r="B62" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -3636,15 +3641,15 @@
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
     </row>
-    <row r="63" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" s="50" customFormat="1"/>
+    <row r="64" spans="1:11" s="50" customFormat="1"/>
+    <row r="65" spans="1:11" s="50" customFormat="1"/>
+    <row r="66" spans="1:11" s="50" customFormat="1">
       <c r="A66" s="51" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="67" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" s="50" customFormat="1">
       <c r="C67" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3682,7 +3687,7 @@
         <v>F 50+</v>
       </c>
     </row>
-    <row r="68" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" s="50" customFormat="1">
       <c r="B68" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3697,7 +3702,7 @@
       <c r="J68" s="4"/>
       <c r="K68" s="4"/>
     </row>
-    <row r="69" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" s="50" customFormat="1">
       <c r="B69" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3712,7 +3717,7 @@
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
     </row>
-    <row r="70" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" s="50" customFormat="1">
       <c r="B70" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3727,7 +3732,7 @@
       <c r="J70" s="4"/>
       <c r="K70" s="4"/>
     </row>
-    <row r="71" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" s="50" customFormat="1">
       <c r="B71" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -3744,7 +3749,7 @@
       <c r="J71" s="4"/>
       <c r="K71" s="4"/>
     </row>
-    <row r="72" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" s="50" customFormat="1">
       <c r="B72" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -3761,7 +3766,7 @@
       <c r="J72" s="4"/>
       <c r="K72" s="4"/>
     </row>
-    <row r="73" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" s="50" customFormat="1">
       <c r="B73" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -3778,7 +3783,7 @@
       </c>
       <c r="K73" s="4"/>
     </row>
-    <row r="74" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" s="50" customFormat="1">
       <c r="B74" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -3795,7 +3800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" s="50" customFormat="1">
       <c r="B75" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -3810,7 +3815,7 @@
       <c r="J75" s="4"/>
       <c r="K75" s="4"/>
     </row>
-    <row r="76" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" s="50" customFormat="1">
       <c r="B76" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -3825,15 +3830,15 @@
       <c r="J76" s="4"/>
       <c r="K76" s="4"/>
     </row>
-    <row r="77" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" s="50" customFormat="1"/>
+    <row r="78" spans="1:11" s="50" customFormat="1"/>
+    <row r="79" spans="1:11" s="50" customFormat="1"/>
+    <row r="80" spans="1:11">
       <c r="A80" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:11">
       <c r="C81" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3871,7 +3876,7 @@
         <v>F 50+</v>
       </c>
     </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:11">
       <c r="B82" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3890,7 +3895,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:11">
       <c r="B83" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3909,7 +3914,7 @@
       </c>
       <c r="K83" s="4"/>
     </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:11">
       <c r="B84" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3924,7 +3929,7 @@
       <c r="J84" s="4"/>
       <c r="K84" s="4"/>
     </row>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:11">
       <c r="B85" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -3939,7 +3944,7 @@
       <c r="J85" s="4"/>
       <c r="K85" s="4"/>
     </row>
-    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:11">
       <c r="B86" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -3954,7 +3959,7 @@
       <c r="J86" s="4"/>
       <c r="K86" s="4"/>
     </row>
-    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:11">
       <c r="B87" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -3969,7 +3974,7 @@
       <c r="J87" s="4"/>
       <c r="K87" s="4"/>
     </row>
-    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:11">
       <c r="B88" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -3984,7 +3989,7 @@
       <c r="J88" s="4"/>
       <c r="K88" s="4"/>
     </row>
-    <row r="89" spans="2:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:11" s="50" customFormat="1">
       <c r="B89" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -3999,7 +4004,7 @@
       <c r="J89" s="4"/>
       <c r="K89" s="4"/>
     </row>
-    <row r="90" spans="2:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:11" s="50" customFormat="1">
       <c r="B90" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -4033,12 +4038,12 @@
       <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="44" t="s">
         <v>56</v>
       </c>
@@ -4047,7 +4052,7 @@
       <c r="D1" s="43"/>
       <c r="E1" s="43"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="43"/>
       <c r="B2" s="43"/>
       <c r="C2" s="46" t="s">
@@ -4060,7 +4065,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="43"/>
       <c r="B3" s="45" t="s">
         <v>57</v>
@@ -4075,7 +4080,7 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="43"/>
       <c r="B4" s="45" t="s">
         <v>58</v>
@@ -4090,7 +4095,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="43"/>
       <c r="B5" s="45" t="s">
         <v>59</v>
@@ -4105,7 +4110,7 @@
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="43"/>
       <c r="B6" s="45" t="s">
         <v>60</v>
@@ -4120,7 +4125,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="43"/>
       <c r="B7" s="45" t="s">
         <v>61</v>
@@ -4135,7 +4140,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="43"/>
       <c r="B8" s="45" t="s">
         <v>62</v>
@@ -4150,7 +4155,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="43"/>
       <c r="B9" s="45" t="s">
         <v>63</v>
@@ -4165,28 +4170,28 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="35"/>
       <c r="B10" s="37"/>
       <c r="C10" s="35"/>
       <c r="D10" s="35"/>
       <c r="E10" s="35"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="35"/>
       <c r="B11" s="37"/>
       <c r="C11" s="35"/>
       <c r="D11" s="35"/>
       <c r="E11" s="35"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="35"/>
       <c r="B12" s="37"/>
       <c r="C12" s="35"/>
       <c r="D12" s="35"/>
       <c r="E12" s="35"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="44" t="s">
         <v>64</v>
       </c>
@@ -4195,7 +4200,7 @@
       <c r="D13" s="43"/>
       <c r="E13" s="43"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="43"/>
       <c r="B14" s="43"/>
       <c r="C14" s="46" t="s">
@@ -4208,7 +4213,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="43"/>
       <c r="B15" s="45" t="s">
         <v>65</v>
@@ -4223,7 +4228,7 @@
         <v>48.02</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="43"/>
       <c r="B16" s="45" t="s">
         <v>66</v>
@@ -4238,7 +4243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="43"/>
       <c r="B17" s="45" t="s">
         <v>67</v>
@@ -4253,7 +4258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="43"/>
       <c r="B18" s="45" t="s">
         <v>68</v>
@@ -4268,7 +4273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="43"/>
       <c r="B19" s="45" t="s">
         <v>69</v>
@@ -4283,7 +4288,7 @@
         <v>6.92</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="43"/>
       <c r="B20" s="45" t="s">
         <v>70</v>
@@ -4298,28 +4303,28 @@
         <v>12.08</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="35"/>
       <c r="B21" s="37"/>
       <c r="C21" s="35"/>
       <c r="D21" s="35"/>
       <c r="E21" s="35"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="35"/>
       <c r="B22" s="37"/>
       <c r="C22" s="35"/>
       <c r="D22" s="35"/>
       <c r="E22" s="35"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="35"/>
       <c r="B23" s="37"/>
       <c r="C23" s="35"/>
       <c r="D23" s="35"/>
       <c r="E23" s="35"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="44" t="s">
         <v>71</v>
       </c>
@@ -4328,7 +4333,7 @@
       <c r="D24" s="43"/>
       <c r="E24" s="43"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="43"/>
       <c r="B25" s="43"/>
       <c r="C25" s="46" t="s">
@@ -4341,7 +4346,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="43"/>
       <c r="B26" s="45" t="s">
         <v>72</v>
@@ -4356,7 +4361,7 @@
         <v>9.76</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="43"/>
       <c r="B27" s="45" t="s">
         <v>67</v>
@@ -4371,7 +4376,7 @@
         <v>1.61</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="43"/>
       <c r="B28" s="45" t="s">
         <v>103</v>
@@ -4386,7 +4391,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="43"/>
       <c r="B29" s="45" t="s">
         <v>73</v>
@@ -4401,7 +4406,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" s="43"/>
       <c r="B30" s="45" t="s">
         <v>74</v>
@@ -4416,28 +4421,28 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" s="35"/>
       <c r="B31" s="37"/>
       <c r="C31" s="35"/>
       <c r="D31" s="35"/>
       <c r="E31" s="35"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="35"/>
       <c r="B32" s="37"/>
       <c r="C32" s="35"/>
       <c r="D32" s="35"/>
       <c r="E32" s="35"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="35"/>
       <c r="B33" s="37"/>
       <c r="C33" s="35"/>
       <c r="D33" s="35"/>
       <c r="E33" s="35"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="44" t="s">
         <v>75</v>
       </c>
@@ -4446,7 +4451,7 @@
       <c r="D34" s="43"/>
       <c r="E34" s="43"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="43"/>
       <c r="B35" s="43"/>
       <c r="C35" s="46" t="s">
@@ -4459,7 +4464,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" s="43"/>
       <c r="B36" s="45" t="s">
         <v>76</v>
@@ -4474,7 +4479,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="43"/>
       <c r="B37" s="45" t="s">
         <v>77</v>
@@ -4489,7 +4494,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="43"/>
       <c r="B38" s="45" t="s">
         <v>78</v>
@@ -4504,7 +4509,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="43"/>
       <c r="B39" s="45" t="s">
         <v>79</v>
@@ -4519,28 +4524,28 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="35"/>
       <c r="B40" s="37"/>
       <c r="C40" s="35"/>
       <c r="D40" s="35"/>
       <c r="E40" s="35"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" s="35"/>
       <c r="B41" s="37"/>
       <c r="C41" s="35"/>
       <c r="D41" s="35"/>
       <c r="E41" s="35"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="35"/>
       <c r="B42" s="37"/>
       <c r="C42" s="35"/>
       <c r="D42" s="35"/>
       <c r="E42" s="35"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="44" t="s">
         <v>80</v>
       </c>
@@ -4549,7 +4554,7 @@
       <c r="D43" s="43"/>
       <c r="E43" s="43"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="43"/>
       <c r="B44" s="43"/>
       <c r="C44" s="46" t="s">
@@ -4562,7 +4567,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="43"/>
       <c r="B45" s="45" t="s">
         <v>65</v>
@@ -4577,7 +4582,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="43"/>
       <c r="B46" s="45" t="s">
         <v>66</v>
@@ -4592,7 +4597,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="43"/>
       <c r="B47" s="45" t="s">
         <v>81</v>
@@ -4607,7 +4612,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" s="43"/>
       <c r="B48" s="45" t="s">
         <v>68</v>
@@ -4622,7 +4627,7 @@
         <v>1.01E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9">
       <c r="A49" s="43"/>
       <c r="B49" s="45" t="s">
         <v>69</v>
@@ -4641,7 +4646,7 @@
       <c r="H49" s="35"/>
       <c r="I49" s="35"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9">
       <c r="A50" s="43"/>
       <c r="B50" s="45" t="s">
         <v>70</v>
@@ -4660,7 +4665,7 @@
       <c r="H50" s="35"/>
       <c r="I50" s="35"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9">
       <c r="A51" s="43"/>
       <c r="B51" s="45" t="s">
         <v>82</v>
@@ -4679,7 +4684,7 @@
       <c r="H51" s="35"/>
       <c r="I51" s="35"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9">
       <c r="A52" s="43"/>
       <c r="B52" s="45" t="s">
         <v>83</v>
@@ -4698,7 +4703,7 @@
       <c r="H52" s="35"/>
       <c r="I52" s="35"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9">
       <c r="A53" s="35"/>
       <c r="B53" s="37"/>
       <c r="C53" s="35"/>
@@ -4709,7 +4714,7 @@
       <c r="H53" s="35"/>
       <c r="I53" s="35"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9">
       <c r="A54" s="35"/>
       <c r="B54" s="37"/>
       <c r="C54" s="35"/>
@@ -4720,7 +4725,7 @@
       <c r="H54" s="35"/>
       <c r="I54" s="35"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9">
       <c r="A55" s="35"/>
       <c r="B55" s="37"/>
       <c r="C55" s="35"/>
@@ -4731,7 +4736,7 @@
       <c r="H55" s="35"/>
       <c r="I55" s="35"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9">
       <c r="A56" s="44" t="s">
         <v>104</v>
       </c>
@@ -4744,7 +4749,7 @@
       <c r="H56" s="35"/>
       <c r="I56" s="35"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9">
       <c r="A57" s="43"/>
       <c r="B57" s="43"/>
       <c r="C57" s="46" t="s">
@@ -4761,7 +4766,7 @@
       <c r="H57" s="35"/>
       <c r="I57" s="35"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9">
       <c r="A58" s="43"/>
       <c r="B58" s="45" t="s">
         <v>84</v>
@@ -4780,7 +4785,7 @@
       <c r="H58" s="39"/>
       <c r="I58" s="39"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9">
       <c r="A59" s="43"/>
       <c r="B59" s="45" t="s">
         <v>85</v>
@@ -4799,7 +4804,7 @@
       <c r="H59" s="39"/>
       <c r="I59" s="39"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9">
       <c r="A60" s="43"/>
       <c r="B60" s="45" t="s">
         <v>86</v>
@@ -4815,7 +4820,7 @@
       </c>
       <c r="F60" s="35"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9">
       <c r="A61" s="43"/>
       <c r="B61" s="45" t="s">
         <v>100</v>
@@ -4834,7 +4839,7 @@
       <c r="H61" s="39"/>
       <c r="I61" s="39"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9">
       <c r="A62" s="43"/>
       <c r="B62" s="45" t="s">
         <v>87</v>
@@ -4853,7 +4858,7 @@
       <c r="H62" s="39"/>
       <c r="I62" s="39"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9">
       <c r="A63" s="43"/>
       <c r="B63" s="45" t="s">
         <v>16</v>
@@ -4872,7 +4877,7 @@
       <c r="H63" s="39"/>
       <c r="I63" s="39"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9">
       <c r="A64" s="43"/>
       <c r="B64" s="45" t="s">
         <v>88</v>
@@ -4891,7 +4896,7 @@
       <c r="H64" s="39"/>
       <c r="I64" s="39"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" s="43"/>
       <c r="B65" s="45" t="s">
         <v>105</v>
@@ -4910,7 +4915,7 @@
       <c r="H65" s="39"/>
       <c r="I65" s="39"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" s="43"/>
       <c r="B66" s="45" t="s">
         <v>106</v>
@@ -4929,7 +4934,7 @@
       <c r="H66" s="35"/>
       <c r="I66" s="35"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" s="35"/>
       <c r="B67" s="37"/>
       <c r="C67" s="35"/>
@@ -4940,7 +4945,7 @@
       <c r="H67" s="35"/>
       <c r="I67" s="35"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="36"/>
       <c r="B68" s="37"/>
       <c r="C68" s="35"/>
@@ -4951,7 +4956,7 @@
       <c r="H68" s="35"/>
       <c r="I68" s="35"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" s="35"/>
       <c r="B69" s="37"/>
       <c r="C69" s="38"/>
@@ -4962,7 +4967,7 @@
       <c r="H69" s="35"/>
       <c r="I69" s="35"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="44" t="s">
         <v>89</v>
       </c>
@@ -4976,7 +4981,7 @@
       <c r="I70" s="35"/>
       <c r="J70" s="24"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" s="43"/>
       <c r="B71" s="43"/>
       <c r="C71" s="46" t="s">
@@ -4994,7 +4999,7 @@
       <c r="I71" s="35"/>
       <c r="J71" s="24"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="43"/>
       <c r="B72" s="45" t="s">
         <v>90</v>
@@ -5014,7 +5019,7 @@
       <c r="I72" s="35"/>
       <c r="J72" s="24"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" s="43"/>
       <c r="B73" s="45" t="s">
         <v>91</v>
@@ -5033,7 +5038,7 @@
       <c r="H73" s="35"/>
       <c r="I73" s="35"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" s="43"/>
       <c r="B74" s="45" t="s">
         <v>92</v>
@@ -5052,7 +5057,7 @@
       <c r="H74" s="35"/>
       <c r="I74" s="35"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" s="43"/>
       <c r="B75" s="45" t="s">
         <v>93</v>
@@ -5071,7 +5076,7 @@
       <c r="H75" s="35"/>
       <c r="I75" s="35"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" s="43"/>
       <c r="B76" s="45" t="s">
         <v>94</v>
@@ -5090,7 +5095,7 @@
       <c r="H76" s="35"/>
       <c r="I76" s="35"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" s="43"/>
       <c r="B77" s="45" t="s">
         <v>95</v>
@@ -5105,7 +5110,7 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" s="43"/>
       <c r="B78" s="45" t="s">
         <v>96</v>
@@ -5138,20 +5143,20 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
@@ -5177,7 +5182,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="B3" s="3">
         <v>1</v>
       </c>
@@ -5206,7 +5211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="B4" s="3">
         <v>2</v>
       </c>
@@ -5235,7 +5240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="B5" s="3">
         <v>3</v>
       </c>
@@ -5264,7 +5269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="B6" s="3">
         <v>4</v>
       </c>
@@ -5293,7 +5298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="B7" s="3">
         <v>5</v>
       </c>
@@ -5322,7 +5327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="B8" s="3">
         <v>6</v>
       </c>
@@ -5351,7 +5356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="B9" s="3">
         <v>7</v>
       </c>
@@ -5380,7 +5385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="50" customFormat="1">
       <c r="B10" s="3">
         <v>8</v>
       </c>
@@ -5409,7 +5414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="50" customFormat="1">
       <c r="B11" s="3">
         <v>9</v>
       </c>
@@ -5457,21 +5462,21 @@
       <selection activeCell="E36" sqref="E36:N36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K1" s="13"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26">
       <c r="D2" s="3">
         <v>2000</v>
       </c>
@@ -5539,7 +5544,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26">
       <c r="B3" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5573,7 +5578,7 @@
       </c>
       <c r="Z3" s="7"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26">
       <c r="B4" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5629,7 +5634,7 @@
       </c>
       <c r="Z4" s="7"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26">
       <c r="B5" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5663,7 +5668,7 @@
       </c>
       <c r="Z5" s="7"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26">
       <c r="B7" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5697,7 +5702,7 @@
       </c>
       <c r="Z7" s="7"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26">
       <c r="B8" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5753,7 +5758,7 @@
       </c>
       <c r="Z8" s="7"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26">
       <c r="B9" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5787,7 +5792,7 @@
       </c>
       <c r="Z9" s="7"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26">
       <c r="B11" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5821,7 +5826,7 @@
       </c>
       <c r="Z11" s="7"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26">
       <c r="B12" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5877,7 +5882,7 @@
       </c>
       <c r="Z12" s="7"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26">
       <c r="B13" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5911,7 +5916,7 @@
       </c>
       <c r="Z13" s="7"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26">
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
@@ -5924,7 +5929,7 @@
       <c r="M14" s="13"/>
       <c r="N14" s="13"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26">
       <c r="B15" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -5958,7 +5963,7 @@
       </c>
       <c r="Z15" s="7"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26">
       <c r="B16" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -6014,7 +6019,7 @@
       </c>
       <c r="Z16" s="7"/>
     </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:26">
       <c r="B17" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -6048,7 +6053,7 @@
       </c>
       <c r="Z17" s="7"/>
     </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:26">
       <c r="B19" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -6082,7 +6087,7 @@
       </c>
       <c r="Z19" s="7"/>
     </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:26">
       <c r="B20" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -6138,7 +6143,7 @@
       </c>
       <c r="Z20" s="7"/>
     </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:26">
       <c r="B21" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -6172,7 +6177,7 @@
       </c>
       <c r="Z21" s="7"/>
     </row>
-    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:26">
       <c r="B23" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -6206,7 +6211,7 @@
       </c>
       <c r="Z23" s="7"/>
     </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:26">
       <c r="B24" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -6262,7 +6267,7 @@
       </c>
       <c r="Z24" s="7"/>
     </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:26">
       <c r="B25" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -6296,7 +6301,7 @@
       </c>
       <c r="Z25" s="7"/>
     </row>
-    <row r="27" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:26">
       <c r="B27" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -6330,7 +6335,7 @@
       </c>
       <c r="Z27" s="7"/>
     </row>
-    <row r="28" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:26">
       <c r="B28" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -6386,7 +6391,7 @@
       </c>
       <c r="Z28" s="7"/>
     </row>
-    <row r="29" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:26">
       <c r="B29" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -6420,7 +6425,7 @@
       </c>
       <c r="Z29" s="7"/>
     </row>
-    <row r="31" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:26" s="50" customFormat="1">
       <c r="B31" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -6454,7 +6459,7 @@
       </c>
       <c r="Z31" s="7"/>
     </row>
-    <row r="32" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:26" s="50" customFormat="1">
       <c r="B32" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -6520,7 +6525,7 @@
       </c>
       <c r="Z32" s="7"/>
     </row>
-    <row r="33" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:26" s="50" customFormat="1">
       <c r="B33" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -6554,8 +6559,8 @@
       </c>
       <c r="Z33" s="7"/>
     </row>
-    <row r="34" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:26" s="50" customFormat="1"/>
+    <row r="35" spans="2:26" s="50" customFormat="1">
       <c r="B35" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -6589,7 +6594,7 @@
       </c>
       <c r="Z35" s="7"/>
     </row>
-    <row r="36" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:26" s="50" customFormat="1">
       <c r="B36" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -6655,7 +6660,7 @@
       </c>
       <c r="Z36" s="7"/>
     </row>
-    <row r="37" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:26" s="50" customFormat="1">
       <c r="B37" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -6689,7 +6694,7 @@
       </c>
       <c r="Z37" s="7"/>
     </row>
-    <row r="38" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="2:26" s="50" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6709,19 +6714,19 @@
       <selection activeCell="Z37" sqref="Z37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="16" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="16" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="8" customWidth="1"/>
-    <col min="26" max="27" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26">
       <c r="D2" s="3">
         <v>2000</v>
       </c>
@@ -6789,7 +6794,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26">
       <c r="B3" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -6829,7 +6834,7 @@
       </c>
       <c r="Z3" s="5"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26">
       <c r="B4" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -6869,7 +6874,7 @@
       </c>
       <c r="Z4" s="5"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26">
       <c r="B5" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -6909,7 +6914,7 @@
       </c>
       <c r="Z5" s="5"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26">
       <c r="B7" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6943,7 +6948,7 @@
       </c>
       <c r="Z7" s="5"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26">
       <c r="B8" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6979,7 +6984,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26">
       <c r="B9" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -7013,7 +7018,7 @@
       </c>
       <c r="Z9" s="5"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26">
       <c r="B11" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7049,7 +7054,7 @@
       </c>
       <c r="Z11" s="5"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26">
       <c r="B12" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7091,7 +7096,7 @@
       </c>
       <c r="Z12" s="5"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26">
       <c r="B13" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7127,7 +7132,7 @@
       </c>
       <c r="Z13" s="5"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26">
       <c r="B15" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -7161,7 +7166,7 @@
       </c>
       <c r="Z15" s="5"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26">
       <c r="B16" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -7197,7 +7202,7 @@
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:26">
       <c r="B17" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -7231,7 +7236,7 @@
       </c>
       <c r="Z17" s="5"/>
     </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:26">
       <c r="B19" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -7265,7 +7270,7 @@
       </c>
       <c r="Z19" s="5"/>
     </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:26">
       <c r="B20" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -7301,7 +7306,7 @@
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:26">
       <c r="B21" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -7335,7 +7340,7 @@
       </c>
       <c r="Z21" s="5"/>
     </row>
-    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:26">
       <c r="B23" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -7369,7 +7374,7 @@
       </c>
       <c r="Z23" s="5"/>
     </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:26">
       <c r="B24" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -7417,7 +7422,7 @@
       </c>
       <c r="Z24" s="5"/>
     </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:26">
       <c r="B25" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -7451,7 +7456,7 @@
       </c>
       <c r="Z25" s="5"/>
     </row>
-    <row r="27" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:26">
       <c r="B27" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -7485,7 +7490,7 @@
       </c>
       <c r="Z27" s="5"/>
     </row>
-    <row r="28" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:26">
       <c r="B28" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -7533,7 +7538,7 @@
       </c>
       <c r="Z28" s="5"/>
     </row>
-    <row r="29" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:26">
       <c r="B29" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -7567,8 +7572,8 @@
       </c>
       <c r="Z29" s="5"/>
     </row>
-    <row r="30" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:26" s="50" customFormat="1"/>
+    <row r="31" spans="2:26" s="50" customFormat="1">
       <c r="B31" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -7602,7 +7607,7 @@
       </c>
       <c r="Z31" s="5"/>
     </row>
-    <row r="32" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:26" s="50" customFormat="1">
       <c r="B32" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -7641,7 +7646,7 @@
         <v>8.4000000000000003E-4</v>
       </c>
     </row>
-    <row r="33" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:26" s="50" customFormat="1">
       <c r="B33" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -7675,8 +7680,8 @@
       </c>
       <c r="Z33" s="5"/>
     </row>
-    <row r="34" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:26" s="50" customFormat="1"/>
+    <row r="35" spans="2:26" s="50" customFormat="1">
       <c r="B35" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -7710,7 +7715,7 @@
       </c>
       <c r="Z35" s="5"/>
     </row>
-    <row r="36" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:26" s="50" customFormat="1">
       <c r="B36" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -7749,7 +7754,7 @@
         <v>1.2899999999999999E-3</v>
       </c>
     </row>
-    <row r="37" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:26" s="50" customFormat="1">
       <c r="B37" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -7802,14 +7807,14 @@
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25">
       <c r="C2" s="3">
         <v>2000</v>
       </c>
@@ -7877,7 +7882,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25">
       <c r="B3" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -7910,7 +7915,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25">
       <c r="B4" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -7943,7 +7948,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25">
       <c r="B5" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7976,7 +7981,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25">
       <c r="B6" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -8009,7 +8014,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25">
       <c r="B7" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -8042,7 +8047,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25">
       <c r="B8" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -8075,7 +8080,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25">
       <c r="B9" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -8108,7 +8113,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" s="50" customFormat="1">
       <c r="B10" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -8141,7 +8146,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" s="50" customFormat="1">
       <c r="B11" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -8174,12 +8179,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25">
       <c r="C16" s="3">
         <v>2000</v>
       </c>
@@ -8247,7 +8252,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25">
       <c r="B17" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -8280,7 +8285,7 @@
       </c>
       <c r="Y17" s="5"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25">
       <c r="B18" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -8313,7 +8318,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25">
       <c r="B19" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -8346,7 +8351,7 @@
       </c>
       <c r="Y19" s="5"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25">
       <c r="B20" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -8379,7 +8384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25">
       <c r="B21" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -8412,7 +8417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25">
       <c r="B22" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -8445,7 +8450,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25">
       <c r="B23" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -8478,7 +8483,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="24" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" s="50" customFormat="1">
       <c r="B24" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -8511,7 +8516,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="25" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" s="50" customFormat="1">
       <c r="B25" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -8544,12 +8549,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25">
       <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25">
       <c r="C30" s="3">
         <v>2000</v>
       </c>
@@ -8617,7 +8622,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25">
       <c r="B31" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -8650,7 +8655,7 @@
       </c>
       <c r="Y31" s="5"/>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25">
       <c r="B32" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -8683,7 +8688,7 @@
       </c>
       <c r="Y32" s="5"/>
     </row>
-    <row r="33" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:25">
       <c r="B33" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -8716,7 +8721,7 @@
       </c>
       <c r="Y33" s="5"/>
     </row>
-    <row r="34" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:25">
       <c r="B34" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -8749,7 +8754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:25">
       <c r="B35" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -8782,7 +8787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:25">
       <c r="B36" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -8815,7 +8820,7 @@
       </c>
       <c r="Y36" s="5"/>
     </row>
-    <row r="37" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:25">
       <c r="B37" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -8848,7 +8853,7 @@
       </c>
       <c r="Y37" s="5"/>
     </row>
-    <row r="38" spans="2:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:25" s="50" customFormat="1">
       <c r="B38" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -8881,7 +8886,7 @@
       </c>
       <c r="Y38" s="5"/>
     </row>
-    <row r="39" spans="2:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:25" s="50" customFormat="1">
       <c r="B39" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -8933,14 +8938,14 @@
       <selection activeCell="Y54" sqref="Y54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25">
       <c r="C2" s="3">
         <v>2000</v>
       </c>
@@ -9008,7 +9013,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25">
       <c r="B3" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -9043,7 +9048,7 @@
       </c>
       <c r="Y3" s="9"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25">
       <c r="B4" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -9080,7 +9085,7 @@
       </c>
       <c r="Y4" s="9"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25">
       <c r="B5" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -9113,7 +9118,7 @@
       </c>
       <c r="Y5" s="9"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25">
       <c r="B6" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -9146,7 +9151,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25">
       <c r="B7" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -9179,7 +9184,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25">
       <c r="B8" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -9216,7 +9221,7 @@
       </c>
       <c r="Y8" s="9"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25">
       <c r="B9" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -9253,7 +9258,7 @@
       </c>
       <c r="Y9" s="9"/>
     </row>
-    <row r="10" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" s="50" customFormat="1">
       <c r="B10" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -9286,7 +9291,7 @@
       </c>
       <c r="Y10" s="9"/>
     </row>
-    <row r="11" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" s="50" customFormat="1">
       <c r="B11" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -9319,12 +9324,12 @@
       </c>
       <c r="Y11" s="9"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25">
       <c r="A15" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25">
       <c r="C16" s="3">
         <v>2000</v>
       </c>
@@ -9392,7 +9397,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25">
       <c r="B17" s="3" t="s">
         <v>36</v>
       </c>
@@ -9424,12 +9429,12 @@
       </c>
       <c r="Y17" s="4"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25">
       <c r="A21" s="34" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25">
       <c r="C22" s="3">
         <v>2000</v>
       </c>
@@ -9497,7 +9502,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25">
       <c r="B23" s="3" t="s">
         <v>25</v>
       </c>
@@ -9545,12 +9550,12 @@
       </c>
       <c r="Y23" s="4"/>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25">
       <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25">
       <c r="C29" s="3">
         <v>2000</v>
       </c>
@@ -9618,7 +9623,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25">
       <c r="B30" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -9651,7 +9656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25">
       <c r="B31" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -9684,7 +9689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25">
       <c r="B32" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -9717,7 +9722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25">
       <c r="B33" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -9750,7 +9755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25">
       <c r="B34" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -9783,7 +9788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25">
       <c r="B35" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -9816,7 +9821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25">
       <c r="B36" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -9849,7 +9854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" s="50" customFormat="1">
       <c r="B37" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -9882,7 +9887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" s="50" customFormat="1">
       <c r="B38" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -9915,12 +9920,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25">
       <c r="A42" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25">
       <c r="C43" s="3">
         <v>2000</v>
       </c>
@@ -9988,7 +9993,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25">
       <c r="B44" s="3" t="s">
         <v>25</v>
       </c>
@@ -10022,12 +10027,12 @@
       </c>
       <c r="Y44" s="4"/>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25">
       <c r="A48" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25">
       <c r="C49" s="3">
         <v>2000</v>
       </c>
@@ -10095,7 +10100,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25">
       <c r="B50" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -10148,7 +10153,7 @@
       </c>
       <c r="Y50" s="8"/>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25">
       <c r="B51" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -10181,7 +10186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25">
       <c r="B52" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -10234,7 +10239,7 @@
       </c>
       <c r="Y52" s="8"/>
     </row>
-    <row r="53" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" s="50" customFormat="1">
       <c r="B53" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -10267,12 +10272,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25">
       <c r="A57" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25">
       <c r="C58" s="3">
         <v>2000</v>
       </c>
@@ -10340,7 +10345,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25">
       <c r="B59" s="3" t="s">
         <v>25</v>
       </c>
@@ -10387,26 +10392,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="10" max="10" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875"/>
-    <col min="13" max="13" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875"/>
-    <col min="15" max="16" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25">
       <c r="C2" s="3">
         <v>2000</v>
       </c>
@@ -10474,7 +10477,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25">
       <c r="B3" s="3" t="s">
         <v>25</v>
       </c>
@@ -10518,12 +10521,12 @@
       </c>
       <c r="Y3" s="8"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25">
       <c r="C8" s="3">
         <v>2000</v>
       </c>
@@ -10591,7 +10594,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25">
       <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
@@ -10625,12 +10628,12 @@
       </c>
       <c r="Y9" s="8"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25">
       <c r="C14" s="3">
         <v>2000</v>
       </c>
@@ -10698,7 +10701,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25">
       <c r="B15" s="3" t="s">
         <v>25</v>
       </c>
@@ -10756,12 +10759,12 @@
       </c>
       <c r="Y15" s="8"/>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35">
       <c r="C20" s="3">
         <v>2000</v>
       </c>
@@ -10829,7 +10832,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35">
       <c r="B21" s="3" t="s">
         <v>25</v>
       </c>
@@ -10887,7 +10890,7 @@
       </c>
       <c r="Y21" s="40"/>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35">
       <c r="A25" s="30" t="s">
         <v>98</v>
       </c>
@@ -10926,7 +10929,7 @@
       <c r="AH25" s="29"/>
       <c r="AI25" s="29"/>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35">
       <c r="A26" s="29"/>
       <c r="B26" s="29"/>
       <c r="C26" s="31">
@@ -11027,7 +11030,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35">
       <c r="A27" s="29"/>
       <c r="B27" s="31" t="s">
         <v>25</v>
@@ -11068,12 +11071,12 @@
       </c>
       <c r="AI27" s="32"/>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35">
       <c r="C31" s="3">
         <v>2000</v>
       </c>
@@ -11141,7 +11144,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35">
       <c r="B32" s="3" t="s">
         <v>25</v>
       </c>
@@ -11199,12 +11202,12 @@
       </c>
       <c r="Y32" s="8"/>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25">
       <c r="A36" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25">
       <c r="C37" s="3">
         <v>2000</v>
       </c>
@@ -11272,7 +11275,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25">
       <c r="B38" s="3" t="s">
         <v>25</v>
       </c>
@@ -11310,10 +11313,10 @@
       </c>
       <c r="Y38" s="8"/>
     </row>
-    <row r="39" spans="1:25" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:25" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:25" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" s="50" customFormat="1" ht="15" customHeight="1"/>
+    <row r="40" spans="1:25" s="50" customFormat="1" ht="15" customHeight="1"/>
+    <row r="41" spans="1:25" s="50" customFormat="1" ht="15" customHeight="1"/>
+    <row r="42" spans="1:25" s="50" customFormat="1">
       <c r="A42" s="66" t="s">
         <v>130</v>
       </c>
@@ -11342,7 +11345,7 @@
       <c r="X42" s="59"/>
       <c r="Y42" s="59"/>
     </row>
-    <row r="43" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" s="50" customFormat="1">
       <c r="A43" s="59"/>
       <c r="B43" s="59"/>
       <c r="C43" s="67">
@@ -11413,7 +11416,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" s="50" customFormat="1">
       <c r="A44" s="59"/>
       <c r="B44" s="67" t="s">
         <v>36</v>
@@ -11444,10 +11447,10 @@
       </c>
       <c r="Y44" s="63"/>
     </row>
-    <row r="45" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" s="50" customFormat="1"/>
+    <row r="46" spans="1:25" s="50" customFormat="1"/>
+    <row r="47" spans="1:25" s="50" customFormat="1"/>
+    <row r="48" spans="1:25" s="50" customFormat="1">
       <c r="A48" s="74" t="s">
         <v>133</v>
       </c>
@@ -11476,7 +11479,7 @@
       <c r="X48" s="70"/>
       <c r="Y48" s="70"/>
     </row>
-    <row r="49" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" s="50" customFormat="1">
       <c r="A49" s="70"/>
       <c r="B49" s="70"/>
       <c r="C49" s="71">
@@ -11547,7 +11550,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25" s="50" customFormat="1">
       <c r="A50" s="70"/>
       <c r="B50" s="71" t="s">
         <v>36</v>
@@ -11578,7 +11581,7 @@
       </c>
       <c r="Y50" s="73"/>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25">
       <c r="A51" s="69"/>
       <c r="B51" s="69"/>
       <c r="C51" s="69"/>
@@ -11605,7 +11608,7 @@
       <c r="X51" s="69"/>
       <c r="Y51" s="69"/>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25">
       <c r="A52" s="69"/>
       <c r="B52" s="69"/>
       <c r="C52" s="69"/>
@@ -11632,7 +11635,7 @@
       <c r="X52" s="69"/>
       <c r="Y52" s="69"/>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25">
       <c r="A53" s="69"/>
       <c r="B53" s="69"/>
       <c r="C53" s="69"/>
@@ -11659,7 +11662,7 @@
       <c r="X53" s="69"/>
       <c r="Y53" s="69"/>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25">
       <c r="A54" s="74" t="s">
         <v>134</v>
       </c>
@@ -11688,7 +11691,7 @@
       <c r="X54" s="70"/>
       <c r="Y54" s="70"/>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25">
       <c r="A55" s="70"/>
       <c r="B55" s="70"/>
       <c r="C55" s="71">
@@ -11759,7 +11762,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25">
       <c r="A56" s="70"/>
       <c r="B56" s="71" t="s">
         <v>36</v>
@@ -11792,6 +11795,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -11803,9 +11811,9 @@
       <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" s="58" t="s">
         <v>108</v>
       </c>
@@ -11834,7 +11842,7 @@
       <c r="X1" s="50"/>
       <c r="Y1" s="50"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25">
       <c r="A2" s="57"/>
       <c r="B2" s="50"/>
       <c r="C2" s="52">
@@ -11905,7 +11913,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25">
       <c r="A3" s="57"/>
       <c r="B3" s="3" t="str">
         <f>Populations!$C$3</f>
@@ -11939,7 +11947,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25">
       <c r="A4" s="57"/>
       <c r="B4" s="3" t="str">
         <f>Populations!$C$4</f>
@@ -11973,7 +11981,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25">
       <c r="A5" s="50"/>
       <c r="B5" s="3" t="str">
         <f>Populations!$C$5</f>
@@ -12007,7 +12015,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25">
       <c r="A6" s="50"/>
       <c r="B6" s="3" t="str">
         <f>Populations!$C$6</f>
@@ -12041,7 +12049,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25">
       <c r="A7" s="50"/>
       <c r="B7" s="3" t="str">
         <f>Populations!$C$7</f>
@@ -12075,7 +12083,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25">
       <c r="B8" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -12108,7 +12116,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25">
       <c r="A9" s="57"/>
       <c r="B9" s="3" t="str">
         <f>Populations!$C$9</f>
@@ -12142,7 +12150,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" s="50" customFormat="1">
       <c r="A10" s="57"/>
       <c r="B10" s="3" t="str">
         <f>Populations!$C$10</f>
@@ -12176,7 +12184,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" s="50" customFormat="1">
       <c r="A11" s="57"/>
       <c r="B11" s="3" t="str">
         <f>Populations!$C$11</f>
@@ -12210,7 +12218,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25">
       <c r="A15" s="58" t="s">
         <v>126</v>
       </c>
@@ -12239,7 +12247,7 @@
       <c r="X15" s="50"/>
       <c r="Y15" s="50"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25">
       <c r="A16" s="57"/>
       <c r="B16" s="50"/>
       <c r="C16" s="52">
@@ -12310,7 +12318,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25">
       <c r="B17" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -12343,7 +12351,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25">
       <c r="A18" s="57"/>
       <c r="B18" s="3" t="str">
         <f>Populations!$C$4</f>
@@ -12377,7 +12385,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25">
       <c r="A19" s="50"/>
       <c r="B19" s="3" t="str">
         <f>Populations!$C$5</f>
@@ -12411,7 +12419,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25">
       <c r="A20" s="50"/>
       <c r="B20" s="3" t="str">
         <f>Populations!$C$6</f>
@@ -12445,7 +12453,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25">
       <c r="A21" s="50"/>
       <c r="B21" s="3" t="str">
         <f>Populations!$C$7</f>
@@ -12479,7 +12487,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25">
       <c r="B22" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -12512,7 +12520,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25">
       <c r="A23" s="50"/>
       <c r="B23" s="3" t="str">
         <f>Populations!$C$9</f>
@@ -12546,7 +12554,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="24" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" s="50" customFormat="1">
       <c r="B24" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -12579,7 +12587,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="25" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" s="50" customFormat="1">
       <c r="B25" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -12612,7 +12620,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25">
       <c r="A29" s="58" t="s">
         <v>109</v>
       </c>
@@ -12641,7 +12649,7 @@
       <c r="X29" s="50"/>
       <c r="Y29" s="50"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25">
       <c r="A30" s="50"/>
       <c r="B30" s="50"/>
       <c r="C30" s="52">
@@ -12712,7 +12720,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25">
       <c r="A31" s="50"/>
       <c r="B31" s="3" t="str">
         <f>Populations!$C$3</f>
@@ -12746,7 +12754,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25">
       <c r="A32" s="50"/>
       <c r="B32" s="3" t="str">
         <f>Populations!$C$4</f>
@@ -12780,7 +12788,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25">
       <c r="A33" s="50"/>
       <c r="B33" s="3" t="str">
         <f>Populations!$C$5</f>
@@ -12814,7 +12822,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25">
       <c r="A34" s="50"/>
       <c r="B34" s="3" t="str">
         <f>Populations!$C$6</f>
@@ -12848,7 +12856,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25">
       <c r="A35" s="50"/>
       <c r="B35" s="3" t="str">
         <f>Populations!$C$7</f>
@@ -12882,7 +12890,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25">
       <c r="A36" s="50"/>
       <c r="B36" s="3" t="str">
         <f>Populations!$C$8</f>
@@ -12916,7 +12924,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25">
       <c r="A37" s="50"/>
       <c r="B37" s="3" t="str">
         <f>Populations!$C$9</f>
@@ -12950,7 +12958,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="38" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" s="50" customFormat="1">
       <c r="B38" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -12983,7 +12991,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="39" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" s="50" customFormat="1">
       <c r="B39" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -13016,7 +13024,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25">
       <c r="A43" s="58" t="s">
         <v>110</v>
       </c>
@@ -13045,7 +13053,7 @@
       <c r="X43" s="50"/>
       <c r="Y43" s="50"/>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25">
       <c r="A44" s="50"/>
       <c r="B44" s="50"/>
       <c r="C44" s="52">
@@ -13116,7 +13124,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25">
       <c r="A45" s="50"/>
       <c r="B45" s="3" t="str">
         <f>Populations!$C$3</f>
@@ -13150,7 +13158,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25">
       <c r="A46" s="50"/>
       <c r="B46" s="3" t="str">
         <f>Populations!$C$4</f>
@@ -13184,7 +13192,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25">
       <c r="A47" s="50"/>
       <c r="B47" s="3" t="str">
         <f>Populations!$C$5</f>
@@ -13218,7 +13226,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25">
       <c r="A48" s="50"/>
       <c r="B48" s="3" t="str">
         <f>Populations!$C$6</f>
@@ -13252,7 +13260,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25">
       <c r="A49" s="50"/>
       <c r="B49" s="3" t="str">
         <f>Populations!$C$7</f>
@@ -13286,7 +13294,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25">
       <c r="A50" s="50"/>
       <c r="B50" s="3" t="str">
         <f>Populations!$C$8</f>
@@ -13320,7 +13328,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25">
       <c r="A51" s="50"/>
       <c r="B51" s="3" t="str">
         <f>Populations!$C$9</f>
@@ -13354,7 +13362,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="52" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" s="50" customFormat="1">
       <c r="B52" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -13387,7 +13395,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="53" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" s="50" customFormat="1">
       <c r="B53" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -13420,7 +13428,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25">
       <c r="A57" s="60" t="s">
         <v>127</v>
       </c>
@@ -13449,7 +13457,7 @@
       <c r="X57" s="59"/>
       <c r="Y57" s="59"/>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25">
       <c r="A58" s="59"/>
       <c r="B58" s="59"/>
       <c r="C58" s="61">
@@ -13520,7 +13528,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25">
       <c r="A59" s="59"/>
       <c r="B59" s="61" t="s">
         <v>36</v>
@@ -13553,7 +13561,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25">
       <c r="A63" s="60" t="s">
         <v>107</v>
       </c>
@@ -13582,7 +13590,7 @@
       <c r="X63" s="59"/>
       <c r="Y63" s="59"/>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:25">
       <c r="A64" s="59"/>
       <c r="B64" s="59"/>
       <c r="C64" s="61">
@@ -13653,7 +13661,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25">
       <c r="A65" s="59"/>
       <c r="B65" s="61" t="s">
         <v>36</v>
@@ -13686,7 +13694,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25">
       <c r="A69" s="60" t="s">
         <v>128</v>
       </c>
@@ -13715,7 +13723,7 @@
       <c r="X69" s="59"/>
       <c r="Y69" s="59"/>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25">
       <c r="A70" s="59"/>
       <c r="B70" s="59"/>
       <c r="C70" s="61">
@@ -13786,7 +13794,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25">
       <c r="A71" s="59"/>
       <c r="B71" s="61" t="s">
         <v>36</v>
@@ -13819,7 +13827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25">
       <c r="A75" s="60" t="s">
         <v>129</v>
       </c>
@@ -13848,7 +13856,7 @@
       <c r="X75" s="59"/>
       <c r="Y75" s="59"/>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25">
       <c r="A76" s="59"/>
       <c r="B76" s="59"/>
       <c r="C76" s="61">
@@ -13919,7 +13927,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:25">
       <c r="A77" s="59"/>
       <c r="B77" s="61" t="s">
         <v>36</v>
@@ -13952,7 +13960,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:25">
       <c r="A81" s="60" t="s">
         <v>131</v>
       </c>
@@ -13981,7 +13989,7 @@
       <c r="X81" s="59"/>
       <c r="Y81" s="59"/>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:25">
       <c r="A82" s="59"/>
       <c r="B82" s="59"/>
       <c r="C82" s="61">
@@ -14052,7 +14060,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:25">
       <c r="A83" s="59"/>
       <c r="B83" s="61" t="s">
         <v>36</v>
@@ -14085,7 +14093,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:25">
       <c r="A87" s="60" t="s">
         <v>132</v>
       </c>
@@ -14114,7 +14122,7 @@
       <c r="X87" s="59"/>
       <c r="Y87" s="59"/>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:25">
       <c r="A88" s="59"/>
       <c r="B88" s="59"/>
       <c r="C88" s="61">
@@ -14185,7 +14193,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:25">
       <c r="A89" s="59"/>
       <c r="B89" s="61" t="s">
         <v>36</v>
@@ -14233,18 +14241,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y91"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="Y52" sqref="Y52:Y53"/>
+    <sheetView tabSelected="1" topLeftCell="C72" workbookViewId="0">
+      <selection activeCell="M91" sqref="M91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25">
       <c r="C2" s="3">
         <v>2000</v>
       </c>
@@ -14312,7 +14320,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25">
       <c r="B3" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -14345,7 +14353,7 @@
       </c>
       <c r="Y3" s="4"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25">
       <c r="B4" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -14378,7 +14386,7 @@
       </c>
       <c r="Y4" s="4"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25">
       <c r="B5" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -14411,7 +14419,7 @@
       </c>
       <c r="Y5" s="4"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25">
       <c r="B6" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -14444,7 +14452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25">
       <c r="B7" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -14477,7 +14485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25">
       <c r="B8" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -14510,7 +14518,7 @@
       </c>
       <c r="Y8" s="4"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25">
       <c r="B9" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -14543,7 +14551,7 @@
       </c>
       <c r="Y9" s="4"/>
     </row>
-    <row r="10" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" s="50" customFormat="1">
       <c r="B10" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -14576,7 +14584,7 @@
       </c>
       <c r="Y10" s="4"/>
     </row>
-    <row r="11" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" s="50" customFormat="1">
       <c r="B11" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -14609,12 +14617,12 @@
       </c>
       <c r="Y11" s="4"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25">
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25">
       <c r="C16" s="3">
         <v>2000</v>
       </c>
@@ -14682,7 +14690,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25">
       <c r="B17" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -14715,7 +14723,7 @@
       </c>
       <c r="Y17" s="4"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25">
       <c r="B18" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -14748,7 +14756,7 @@
       </c>
       <c r="Y18" s="4"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25">
       <c r="B19" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -14781,7 +14789,7 @@
       </c>
       <c r="Y19" s="4"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25">
       <c r="B20" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -14814,7 +14822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25">
       <c r="B21" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -14847,7 +14855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25">
       <c r="B22" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -14880,7 +14888,7 @@
       </c>
       <c r="Y22" s="4"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25">
       <c r="B23" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -14913,7 +14921,7 @@
       </c>
       <c r="Y23" s="4"/>
     </row>
-    <row r="24" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" s="50" customFormat="1">
       <c r="B24" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -14946,7 +14954,7 @@
       </c>
       <c r="Y24" s="4"/>
     </row>
-    <row r="25" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" s="50" customFormat="1">
       <c r="B25" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -14979,12 +14987,12 @@
       </c>
       <c r="Y25" s="4"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25">
       <c r="A29" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25">
       <c r="C30" s="3">
         <v>2000</v>
       </c>
@@ -15052,7 +15060,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25">
       <c r="B31" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -15085,7 +15093,7 @@
       </c>
       <c r="Y31" s="4"/>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25">
       <c r="B32" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -15118,7 +15126,7 @@
       </c>
       <c r="Y32" s="4"/>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25">
       <c r="B33" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -15151,7 +15159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25">
       <c r="B34" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -15184,7 +15192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25">
       <c r="B35" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -15217,7 +15225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25">
       <c r="B36" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -15250,7 +15258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25">
       <c r="B37" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -15283,7 +15291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" s="50" customFormat="1">
       <c r="B38" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -15316,7 +15324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" s="50" customFormat="1">
       <c r="B39" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -15349,12 +15357,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25">
       <c r="A43" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25">
       <c r="C44" s="3">
         <v>2000</v>
       </c>
@@ -15422,7 +15430,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25">
       <c r="B45" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -15455,7 +15463,7 @@
       </c>
       <c r="Y45" s="9"/>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25">
       <c r="B46" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -15488,7 +15496,7 @@
       </c>
       <c r="Y46" s="9"/>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25">
       <c r="B47" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -15521,7 +15529,7 @@
       </c>
       <c r="Y47" s="9"/>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25">
       <c r="B48" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -15554,7 +15562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25">
       <c r="B49" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -15587,7 +15595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25">
       <c r="B50" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -15620,7 +15628,7 @@
       </c>
       <c r="Y50" s="9"/>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25">
       <c r="B51" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -15653,7 +15661,7 @@
       </c>
       <c r="Y51" s="9"/>
     </row>
-    <row r="52" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" s="50" customFormat="1">
       <c r="B52" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -15686,7 +15694,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" s="50" customFormat="1">
       <c r="B53" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -15719,12 +15727,12 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25">
       <c r="A57" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25">
       <c r="C58" s="3">
         <v>2000</v>
       </c>
@@ -15792,7 +15800,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25">
       <c r="B59" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -15825,7 +15833,7 @@
       </c>
       <c r="Y59" s="9"/>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25">
       <c r="B60" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -15862,7 +15870,7 @@
       </c>
       <c r="Y60" s="9"/>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25">
       <c r="B61" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -15895,7 +15903,7 @@
       </c>
       <c r="Y61" s="9"/>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25">
       <c r="B62" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -15928,7 +15936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25">
       <c r="B63" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -15961,7 +15969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:25">
       <c r="B64" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -15998,7 +16006,7 @@
       </c>
       <c r="Y64" s="9"/>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25">
       <c r="B65" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -16035,7 +16043,7 @@
       </c>
       <c r="Y65" s="9"/>
     </row>
-    <row r="66" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" s="50" customFormat="1">
       <c r="B66" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -16068,7 +16076,7 @@
       </c>
       <c r="Y66" s="9"/>
     </row>
-    <row r="67" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" s="50" customFormat="1">
       <c r="B67" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -16101,12 +16109,12 @@
       </c>
       <c r="Y67" s="9"/>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25">
       <c r="A71" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25">
       <c r="C72" s="3">
         <v>2000</v>
       </c>
@@ -16174,7 +16182,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:25">
       <c r="B73" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -16209,7 +16217,7 @@
       </c>
       <c r="Y73" s="9"/>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:25">
       <c r="B74" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -16242,7 +16250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25">
       <c r="B75" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -16275,7 +16283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25">
       <c r="B76" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -16308,7 +16316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:25">
       <c r="B77" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -16341,7 +16349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:25">
       <c r="B78" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -16374,7 +16382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25">
       <c r="B79" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -16407,7 +16415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:25" s="50" customFormat="1">
       <c r="B80" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -16440,7 +16448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:25" s="50" customFormat="1">
       <c r="B81" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -16473,12 +16481,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:25">
       <c r="A85" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:25">
       <c r="C86" s="3">
         <v>2000</v>
       </c>
@@ -16546,7 +16554,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:25">
       <c r="B87" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -16562,7 +16570,7 @@
       <c r="K87" s="9"/>
       <c r="L87" s="9"/>
       <c r="M87" s="9">
-        <v>0.97</v>
+        <v>0.85</v>
       </c>
       <c r="N87" s="9"/>
       <c r="O87" s="9"/>
@@ -16579,7 +16587,7 @@
       </c>
       <c r="Y87" s="9"/>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:25">
       <c r="B88" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -16595,7 +16603,7 @@
       <c r="K88" s="9"/>
       <c r="L88" s="9"/>
       <c r="M88" s="9">
-        <v>0.97</v>
+        <v>0.85</v>
       </c>
       <c r="N88" s="9"/>
       <c r="O88" s="9"/>
@@ -16612,7 +16620,7 @@
       </c>
       <c r="Y88" s="9"/>
     </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:25">
       <c r="B89" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -16628,7 +16636,7 @@
       <c r="K89" s="9"/>
       <c r="L89" s="9"/>
       <c r="M89" s="9">
-        <v>0.97</v>
+        <v>0.85</v>
       </c>
       <c r="N89" s="9"/>
       <c r="O89" s="9"/>
@@ -16645,7 +16653,7 @@
       </c>
       <c r="Y89" s="9"/>
     </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:25">
       <c r="B90" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -16661,7 +16669,7 @@
       <c r="K90" s="9"/>
       <c r="L90" s="9"/>
       <c r="M90" s="9">
-        <v>0.97</v>
+        <v>0.85</v>
       </c>
       <c r="N90" s="9"/>
       <c r="O90" s="9"/>
@@ -16678,7 +16686,7 @@
       </c>
       <c r="Y90" s="9"/>
     </row>
-    <row r="91" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:25" s="50" customFormat="1">
       <c r="B91" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -16694,7 +16702,7 @@
       <c r="K91" s="9"/>
       <c r="L91" s="9"/>
       <c r="M91" s="9">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="N91" s="9"/>
       <c r="O91" s="9"/>

</xml_diff>

<commit_message>
weird bug in generalized.xlsx
</commit_message>
<xml_diff>
--- a/tests/generalized.xlsx
+++ b/tests/generalized.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="1480" windowWidth="19420" windowHeight="10960" tabRatio="901" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="2205" yWindow="1485" windowWidth="19425" windowHeight="10965" tabRatio="901" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Partnerships &amp; transitions" sheetId="10" r:id="rId11"/>
     <sheet name="Constants" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -477,9 +477,6 @@
     <t>F 50+</t>
   </si>
   <si>
-    <t>Males 15-49</t>
-  </si>
-  <si>
     <t>Females 15-49</t>
   </si>
   <si>
@@ -518,14 +515,17 @@
   <si>
     <t>PLHIV in care on treatment (%)</t>
   </si>
+  <si>
+    <t>Males 15-49kk</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="7">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="#,##0_ ;\-#,##0\ "/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
@@ -749,12 +749,12 @@
   </borders>
   <cellStyleXfs count="306">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -817,7 +817,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1091,7 +1091,7 @@
     <xf numFmtId="166" fontId="0" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1850,34 +1850,34 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.33203125" customWidth="1"/>
+    <col min="1" max="1" width="89.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="75" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="76"/>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="76"/>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="25"/>
     </row>
-    <row r="5" spans="1:1" ht="28">
+    <row r="5" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="25"/>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>97</v>
       </c>
@@ -1904,14 +1904,14 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C2" s="3">
         <v>2000</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2012,7 +2012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2045,7 +2045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2078,7 +2078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -2111,7 +2111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -2144,7 +2144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -2177,7 +2177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -2210,7 +2210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:25" s="50" customFormat="1">
+    <row r="10" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -2243,7 +2243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:25" s="50" customFormat="1">
+    <row r="11" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -2276,12 +2276,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C16" s="3">
         <v>2000</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2382,7 +2382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2415,7 +2415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2448,7 +2448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -2481,7 +2481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -2514,7 +2514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -2547,7 +2547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -2580,7 +2580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:25" s="50" customFormat="1">
+    <row r="24" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -2613,7 +2613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:25" s="50" customFormat="1">
+    <row r="25" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -2646,12 +2646,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C30" s="3">
         <v>2000</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>36</v>
       </c>
@@ -2770,18 +2770,18 @@
       <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="11" width="12.6640625" style="50" customWidth="1"/>
+    <col min="3" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="11" width="12.7109375" style="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C2" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2819,7 +2819,7 @@
         <v>F 50+</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2834,7 +2834,7 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2855,7 +2855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2872,7 +2872,7 @@
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -2887,7 +2887,7 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -2902,7 +2902,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -2923,7 +2923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -2938,7 +2938,7 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:11" s="50" customFormat="1">
+    <row r="10" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -2959,7 +2959,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="50" customFormat="1">
+    <row r="11" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -2974,12 +2974,12 @@
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3017,7 +3017,7 @@
         <v>F 50+</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3032,7 +3032,7 @@
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3053,7 +3053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3070,7 +3070,7 @@
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -3085,7 +3085,7 @@
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -3100,7 +3100,7 @@
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -3121,7 +3121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -3136,7 +3136,7 @@
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="1:11" s="50" customFormat="1">
+    <row r="24" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -3157,7 +3157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="50" customFormat="1">
+    <row r="25" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -3172,12 +3172,12 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C30" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3215,7 +3215,7 @@
         <v>F 50+</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3230,7 +3230,7 @@
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3247,7 +3247,7 @@
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3262,7 +3262,7 @@
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -3277,7 +3277,7 @@
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -3292,7 +3292,7 @@
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -3307,7 +3307,7 @@
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -3322,7 +3322,7 @@
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
     </row>
-    <row r="38" spans="1:11" s="50" customFormat="1">
+    <row r="38" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -3337,7 +3337,7 @@
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
     </row>
-    <row r="39" spans="1:11" s="50" customFormat="1">
+    <row r="39" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -3352,12 +3352,12 @@
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C44" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3395,7 +3395,7 @@
         <v>F 50+</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3410,7 +3410,7 @@
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3425,7 +3425,7 @@
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3440,7 +3440,7 @@
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -3455,7 +3455,7 @@
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -3470,7 +3470,7 @@
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -3485,7 +3485,7 @@
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -3500,7 +3500,7 @@
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
     </row>
-    <row r="52" spans="1:11" s="50" customFormat="1">
+    <row r="52" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -3515,7 +3515,7 @@
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
     </row>
-    <row r="53" spans="1:11" s="50" customFormat="1">
+    <row r="53" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -3530,12 +3530,12 @@
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
     </row>
-    <row r="57" spans="1:11" s="50" customFormat="1">
+    <row r="57" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="51" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:11" s="50" customFormat="1">
+    <row r="58" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C58" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3573,7 +3573,7 @@
         <v>F 50+</v>
       </c>
     </row>
-    <row r="59" spans="1:11" s="50" customFormat="1">
+    <row r="59" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3592,7 +3592,7 @@
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
     </row>
-    <row r="60" spans="1:11" s="50" customFormat="1">
+    <row r="60" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -3607,7 +3607,7 @@
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
     </row>
-    <row r="61" spans="1:11" s="50" customFormat="1">
+    <row r="61" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -3626,7 +3626,7 @@
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
     </row>
-    <row r="62" spans="1:11" s="50" customFormat="1">
+    <row r="62" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -3641,15 +3641,15 @@
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
     </row>
-    <row r="63" spans="1:11" s="50" customFormat="1"/>
-    <row r="64" spans="1:11" s="50" customFormat="1"/>
-    <row r="65" spans="1:11" s="50" customFormat="1"/>
-    <row r="66" spans="1:11" s="50" customFormat="1">
+    <row r="63" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="51" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" s="50" customFormat="1">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C67" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3687,7 +3687,7 @@
         <v>F 50+</v>
       </c>
     </row>
-    <row r="68" spans="1:11" s="50" customFormat="1">
+    <row r="68" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3702,7 +3702,7 @@
       <c r="J68" s="4"/>
       <c r="K68" s="4"/>
     </row>
-    <row r="69" spans="1:11" s="50" customFormat="1">
+    <row r="69" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3717,7 +3717,7 @@
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
     </row>
-    <row r="70" spans="1:11" s="50" customFormat="1">
+    <row r="70" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3732,7 +3732,7 @@
       <c r="J70" s="4"/>
       <c r="K70" s="4"/>
     </row>
-    <row r="71" spans="1:11" s="50" customFormat="1">
+    <row r="71" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -3749,7 +3749,7 @@
       <c r="J71" s="4"/>
       <c r="K71" s="4"/>
     </row>
-    <row r="72" spans="1:11" s="50" customFormat="1">
+    <row r="72" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -3766,7 +3766,7 @@
       <c r="J72" s="4"/>
       <c r="K72" s="4"/>
     </row>
-    <row r="73" spans="1:11" s="50" customFormat="1">
+    <row r="73" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -3783,7 +3783,7 @@
       </c>
       <c r="K73" s="4"/>
     </row>
-    <row r="74" spans="1:11" s="50" customFormat="1">
+    <row r="74" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -3800,7 +3800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:11" s="50" customFormat="1">
+    <row r="75" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -3815,7 +3815,7 @@
       <c r="J75" s="4"/>
       <c r="K75" s="4"/>
     </row>
-    <row r="76" spans="1:11" s="50" customFormat="1">
+    <row r="76" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -3830,15 +3830,15 @@
       <c r="J76" s="4"/>
       <c r="K76" s="4"/>
     </row>
-    <row r="77" spans="1:11" s="50" customFormat="1"/>
-    <row r="78" spans="1:11" s="50" customFormat="1"/>
-    <row r="79" spans="1:11" s="50" customFormat="1"/>
-    <row r="80" spans="1:11">
+    <row r="77" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="81" spans="2:11">
+    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C81" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3876,7 +3876,7 @@
         <v>F 50+</v>
       </c>
     </row>
-    <row r="82" spans="2:11">
+    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3895,7 +3895,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="2:11">
+    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B83" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3914,7 +3914,7 @@
       </c>
       <c r="K83" s="4"/>
     </row>
-    <row r="84" spans="2:11">
+    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B84" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3929,7 +3929,7 @@
       <c r="J84" s="4"/>
       <c r="K84" s="4"/>
     </row>
-    <row r="85" spans="2:11">
+    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B85" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -3944,7 +3944,7 @@
       <c r="J85" s="4"/>
       <c r="K85" s="4"/>
     </row>
-    <row r="86" spans="2:11">
+    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B86" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -3959,7 +3959,7 @@
       <c r="J86" s="4"/>
       <c r="K86" s="4"/>
     </row>
-    <row r="87" spans="2:11">
+    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -3974,7 +3974,7 @@
       <c r="J87" s="4"/>
       <c r="K87" s="4"/>
     </row>
-    <row r="88" spans="2:11">
+    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B88" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -3989,7 +3989,7 @@
       <c r="J88" s="4"/>
       <c r="K88" s="4"/>
     </row>
-    <row r="89" spans="2:11" s="50" customFormat="1">
+    <row r="89" spans="2:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B89" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -4004,7 +4004,7 @@
       <c r="J89" s="4"/>
       <c r="K89" s="4"/>
     </row>
-    <row r="90" spans="2:11" s="50" customFormat="1">
+    <row r="90" spans="2:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B90" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -4038,12 +4038,12 @@
       <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
         <v>56</v>
       </c>
@@ -4052,7 +4052,7 @@
       <c r="D1" s="43"/>
       <c r="E1" s="43"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="43"/>
       <c r="B2" s="43"/>
       <c r="C2" s="46" t="s">
@@ -4065,7 +4065,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="43"/>
       <c r="B3" s="45" t="s">
         <v>57</v>
@@ -4080,7 +4080,7 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="43"/>
       <c r="B4" s="45" t="s">
         <v>58</v>
@@ -4095,7 +4095,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="43"/>
       <c r="B5" s="45" t="s">
         <v>59</v>
@@ -4110,7 +4110,7 @@
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="43"/>
       <c r="B6" s="45" t="s">
         <v>60</v>
@@ -4125,7 +4125,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="43"/>
       <c r="B7" s="45" t="s">
         <v>61</v>
@@ -4140,7 +4140,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="43"/>
       <c r="B8" s="45" t="s">
         <v>62</v>
@@ -4155,7 +4155,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="43"/>
       <c r="B9" s="45" t="s">
         <v>63</v>
@@ -4170,28 +4170,28 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="35"/>
       <c r="B10" s="37"/>
       <c r="C10" s="35"/>
       <c r="D10" s="35"/>
       <c r="E10" s="35"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="35"/>
       <c r="B11" s="37"/>
       <c r="C11" s="35"/>
       <c r="D11" s="35"/>
       <c r="E11" s="35"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="35"/>
       <c r="B12" s="37"/>
       <c r="C12" s="35"/>
       <c r="D12" s="35"/>
       <c r="E12" s="35"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="s">
         <v>64</v>
       </c>
@@ -4200,7 +4200,7 @@
       <c r="D13" s="43"/>
       <c r="E13" s="43"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="43"/>
       <c r="B14" s="43"/>
       <c r="C14" s="46" t="s">
@@ -4213,7 +4213,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="43"/>
       <c r="B15" s="45" t="s">
         <v>65</v>
@@ -4228,7 +4228,7 @@
         <v>48.02</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="43"/>
       <c r="B16" s="45" t="s">
         <v>66</v>
@@ -4243,7 +4243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="43"/>
       <c r="B17" s="45" t="s">
         <v>67</v>
@@ -4258,7 +4258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="43"/>
       <c r="B18" s="45" t="s">
         <v>68</v>
@@ -4273,7 +4273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="43"/>
       <c r="B19" s="45" t="s">
         <v>69</v>
@@ -4288,7 +4288,7 @@
         <v>6.92</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="43"/>
       <c r="B20" s="45" t="s">
         <v>70</v>
@@ -4303,28 +4303,28 @@
         <v>12.08</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="35"/>
       <c r="B21" s="37"/>
       <c r="C21" s="35"/>
       <c r="D21" s="35"/>
       <c r="E21" s="35"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="35"/>
       <c r="B22" s="37"/>
       <c r="C22" s="35"/>
       <c r="D22" s="35"/>
       <c r="E22" s="35"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="35"/>
       <c r="B23" s="37"/>
       <c r="C23" s="35"/>
       <c r="D23" s="35"/>
       <c r="E23" s="35"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="44" t="s">
         <v>71</v>
       </c>
@@ -4333,7 +4333,7 @@
       <c r="D24" s="43"/>
       <c r="E24" s="43"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="43"/>
       <c r="B25" s="43"/>
       <c r="C25" s="46" t="s">
@@ -4346,7 +4346,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="43"/>
       <c r="B26" s="45" t="s">
         <v>72</v>
@@ -4361,7 +4361,7 @@
         <v>9.76</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="43"/>
       <c r="B27" s="45" t="s">
         <v>67</v>
@@ -4376,7 +4376,7 @@
         <v>1.61</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="43"/>
       <c r="B28" s="45" t="s">
         <v>103</v>
@@ -4391,7 +4391,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="43"/>
       <c r="B29" s="45" t="s">
         <v>73</v>
@@ -4406,7 +4406,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="43"/>
       <c r="B30" s="45" t="s">
         <v>74</v>
@@ -4421,28 +4421,28 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="35"/>
       <c r="B31" s="37"/>
       <c r="C31" s="35"/>
       <c r="D31" s="35"/>
       <c r="E31" s="35"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="35"/>
       <c r="B32" s="37"/>
       <c r="C32" s="35"/>
       <c r="D32" s="35"/>
       <c r="E32" s="35"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="35"/>
       <c r="B33" s="37"/>
       <c r="C33" s="35"/>
       <c r="D33" s="35"/>
       <c r="E33" s="35"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="44" t="s">
         <v>75</v>
       </c>
@@ -4451,7 +4451,7 @@
       <c r="D34" s="43"/>
       <c r="E34" s="43"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="43"/>
       <c r="B35" s="43"/>
       <c r="C35" s="46" t="s">
@@ -4464,7 +4464,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="43"/>
       <c r="B36" s="45" t="s">
         <v>76</v>
@@ -4479,7 +4479,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="43"/>
       <c r="B37" s="45" t="s">
         <v>77</v>
@@ -4494,7 +4494,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="43"/>
       <c r="B38" s="45" t="s">
         <v>78</v>
@@ -4509,7 +4509,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="43"/>
       <c r="B39" s="45" t="s">
         <v>79</v>
@@ -4524,28 +4524,28 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="35"/>
       <c r="B40" s="37"/>
       <c r="C40" s="35"/>
       <c r="D40" s="35"/>
       <c r="E40" s="35"/>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="35"/>
       <c r="B41" s="37"/>
       <c r="C41" s="35"/>
       <c r="D41" s="35"/>
       <c r="E41" s="35"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="35"/>
       <c r="B42" s="37"/>
       <c r="C42" s="35"/>
       <c r="D42" s="35"/>
       <c r="E42" s="35"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="44" t="s">
         <v>80</v>
       </c>
@@ -4554,7 +4554,7 @@
       <c r="D43" s="43"/>
       <c r="E43" s="43"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="43"/>
       <c r="B44" s="43"/>
       <c r="C44" s="46" t="s">
@@ -4567,7 +4567,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="43"/>
       <c r="B45" s="45" t="s">
         <v>65</v>
@@ -4582,7 +4582,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="43"/>
       <c r="B46" s="45" t="s">
         <v>66</v>
@@ -4597,7 +4597,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="43"/>
       <c r="B47" s="45" t="s">
         <v>81</v>
@@ -4612,7 +4612,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="43"/>
       <c r="B48" s="45" t="s">
         <v>68</v>
@@ -4627,7 +4627,7 @@
         <v>1.01E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="43"/>
       <c r="B49" s="45" t="s">
         <v>69</v>
@@ -4646,7 +4646,7 @@
       <c r="H49" s="35"/>
       <c r="I49" s="35"/>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="43"/>
       <c r="B50" s="45" t="s">
         <v>70</v>
@@ -4665,7 +4665,7 @@
       <c r="H50" s="35"/>
       <c r="I50" s="35"/>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="43"/>
       <c r="B51" s="45" t="s">
         <v>82</v>
@@ -4684,7 +4684,7 @@
       <c r="H51" s="35"/>
       <c r="I51" s="35"/>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="43"/>
       <c r="B52" s="45" t="s">
         <v>83</v>
@@ -4703,7 +4703,7 @@
       <c r="H52" s="35"/>
       <c r="I52" s="35"/>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="35"/>
       <c r="B53" s="37"/>
       <c r="C53" s="35"/>
@@ -4714,7 +4714,7 @@
       <c r="H53" s="35"/>
       <c r="I53" s="35"/>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="35"/>
       <c r="B54" s="37"/>
       <c r="C54" s="35"/>
@@ -4725,7 +4725,7 @@
       <c r="H54" s="35"/>
       <c r="I54" s="35"/>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="35"/>
       <c r="B55" s="37"/>
       <c r="C55" s="35"/>
@@ -4736,7 +4736,7 @@
       <c r="H55" s="35"/>
       <c r="I55" s="35"/>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="44" t="s">
         <v>104</v>
       </c>
@@ -4749,7 +4749,7 @@
       <c r="H56" s="35"/>
       <c r="I56" s="35"/>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="43"/>
       <c r="B57" s="43"/>
       <c r="C57" s="46" t="s">
@@ -4766,7 +4766,7 @@
       <c r="H57" s="35"/>
       <c r="I57" s="35"/>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="43"/>
       <c r="B58" s="45" t="s">
         <v>84</v>
@@ -4785,7 +4785,7 @@
       <c r="H58" s="39"/>
       <c r="I58" s="39"/>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="43"/>
       <c r="B59" s="45" t="s">
         <v>85</v>
@@ -4804,7 +4804,7 @@
       <c r="H59" s="39"/>
       <c r="I59" s="39"/>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="43"/>
       <c r="B60" s="45" t="s">
         <v>86</v>
@@ -4820,7 +4820,7 @@
       </c>
       <c r="F60" s="35"/>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="43"/>
       <c r="B61" s="45" t="s">
         <v>100</v>
@@ -4839,7 +4839,7 @@
       <c r="H61" s="39"/>
       <c r="I61" s="39"/>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="43"/>
       <c r="B62" s="45" t="s">
         <v>87</v>
@@ -4858,7 +4858,7 @@
       <c r="H62" s="39"/>
       <c r="I62" s="39"/>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="43"/>
       <c r="B63" s="45" t="s">
         <v>16</v>
@@ -4877,7 +4877,7 @@
       <c r="H63" s="39"/>
       <c r="I63" s="39"/>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="43"/>
       <c r="B64" s="45" t="s">
         <v>88</v>
@@ -4896,7 +4896,7 @@
       <c r="H64" s="39"/>
       <c r="I64" s="39"/>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="43"/>
       <c r="B65" s="45" t="s">
         <v>105</v>
@@ -4915,7 +4915,7 @@
       <c r="H65" s="39"/>
       <c r="I65" s="39"/>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="43"/>
       <c r="B66" s="45" t="s">
         <v>106</v>
@@ -4934,7 +4934,7 @@
       <c r="H66" s="35"/>
       <c r="I66" s="35"/>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="35"/>
       <c r="B67" s="37"/>
       <c r="C67" s="35"/>
@@ -4945,7 +4945,7 @@
       <c r="H67" s="35"/>
       <c r="I67" s="35"/>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="36"/>
       <c r="B68" s="37"/>
       <c r="C68" s="35"/>
@@ -4956,7 +4956,7 @@
       <c r="H68" s="35"/>
       <c r="I68" s="35"/>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="35"/>
       <c r="B69" s="37"/>
       <c r="C69" s="38"/>
@@ -4967,7 +4967,7 @@
       <c r="H69" s="35"/>
       <c r="I69" s="35"/>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="44" t="s">
         <v>89</v>
       </c>
@@ -4981,7 +4981,7 @@
       <c r="I70" s="35"/>
       <c r="J70" s="24"/>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="43"/>
       <c r="B71" s="43"/>
       <c r="C71" s="46" t="s">
@@ -4999,7 +4999,7 @@
       <c r="I71" s="35"/>
       <c r="J71" s="24"/>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="43"/>
       <c r="B72" s="45" t="s">
         <v>90</v>
@@ -5019,7 +5019,7 @@
       <c r="I72" s="35"/>
       <c r="J72" s="24"/>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="43"/>
       <c r="B73" s="45" t="s">
         <v>91</v>
@@ -5038,7 +5038,7 @@
       <c r="H73" s="35"/>
       <c r="I73" s="35"/>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="43"/>
       <c r="B74" s="45" t="s">
         <v>92</v>
@@ -5057,7 +5057,7 @@
       <c r="H74" s="35"/>
       <c r="I74" s="35"/>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="43"/>
       <c r="B75" s="45" t="s">
         <v>93</v>
@@ -5076,7 +5076,7 @@
       <c r="H75" s="35"/>
       <c r="I75" s="35"/>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="43"/>
       <c r="B76" s="45" t="s">
         <v>94</v>
@@ -5095,7 +5095,7 @@
       <c r="H76" s="35"/>
       <c r="I76" s="35"/>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="43"/>
       <c r="B77" s="45" t="s">
         <v>95</v>
@@ -5110,7 +5110,7 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="43"/>
       <c r="B78" s="45" t="s">
         <v>96</v>
@@ -5139,24 +5139,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="40.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
@@ -5182,7 +5182,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
         <v>1</v>
       </c>
@@ -5211,7 +5211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>2</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>3</v>
       </c>
@@ -5269,9 +5269,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>101</v>
@@ -5298,9 +5298,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>102</v>
@@ -5327,7 +5327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>6</v>
       </c>
@@ -5335,7 +5335,7 @@
         <v>117</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>9</v>
@@ -5356,7 +5356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <v>7</v>
       </c>
@@ -5364,7 +5364,7 @@
         <v>118</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>8</v>
@@ -5385,7 +5385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="50" customFormat="1">
+    <row r="10" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>8</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>119</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>9</v>
@@ -5414,7 +5414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="50" customFormat="1">
+    <row r="11" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <v>9</v>
       </c>
@@ -5422,7 +5422,7 @@
         <v>120</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>8</v>
@@ -5462,21 +5462,21 @@
       <selection activeCell="E36" sqref="E36:N36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="12" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K1" s="13"/>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D2" s="3">
         <v>2000</v>
       </c>
@@ -5544,7 +5544,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5578,7 +5578,7 @@
       </c>
       <c r="Z3" s="7"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5634,7 +5634,7 @@
       </c>
       <c r="Z4" s="7"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5668,7 +5668,7 @@
       </c>
       <c r="Z5" s="7"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5702,7 +5702,7 @@
       </c>
       <c r="Z7" s="7"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5758,7 +5758,7 @@
       </c>
       <c r="Z8" s="7"/>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5792,7 +5792,7 @@
       </c>
       <c r="Z9" s="7"/>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5826,7 +5826,7 @@
       </c>
       <c r="Z11" s="7"/>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5882,7 +5882,7 @@
       </c>
       <c r="Z12" s="7"/>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5916,7 +5916,7 @@
       </c>
       <c r="Z13" s="7"/>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
@@ -5929,7 +5929,7 @@
       <c r="M14" s="13"/>
       <c r="N14" s="13"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -5963,7 +5963,7 @@
       </c>
       <c r="Z15" s="7"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -6019,7 +6019,7 @@
       </c>
       <c r="Z16" s="7"/>
     </row>
-    <row r="17" spans="2:26">
+    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -6053,7 +6053,7 @@
       </c>
       <c r="Z17" s="7"/>
     </row>
-    <row r="19" spans="2:26">
+    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -6087,7 +6087,7 @@
       </c>
       <c r="Z19" s="7"/>
     </row>
-    <row r="20" spans="2:26">
+    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -6143,7 +6143,7 @@
       </c>
       <c r="Z20" s="7"/>
     </row>
-    <row r="21" spans="2:26">
+    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -6177,7 +6177,7 @@
       </c>
       <c r="Z21" s="7"/>
     </row>
-    <row r="23" spans="2:26">
+    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -6211,7 +6211,7 @@
       </c>
       <c r="Z23" s="7"/>
     </row>
-    <row r="24" spans="2:26">
+    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -6267,7 +6267,7 @@
       </c>
       <c r="Z24" s="7"/>
     </row>
-    <row r="25" spans="2:26">
+    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -6301,7 +6301,7 @@
       </c>
       <c r="Z25" s="7"/>
     </row>
-    <row r="27" spans="2:26">
+    <row r="27" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -6335,7 +6335,7 @@
       </c>
       <c r="Z27" s="7"/>
     </row>
-    <row r="28" spans="2:26">
+    <row r="28" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -6391,7 +6391,7 @@
       </c>
       <c r="Z28" s="7"/>
     </row>
-    <row r="29" spans="2:26">
+    <row r="29" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -6425,7 +6425,7 @@
       </c>
       <c r="Z29" s="7"/>
     </row>
-    <row r="31" spans="2:26" s="50" customFormat="1">
+    <row r="31" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -6459,7 +6459,7 @@
       </c>
       <c r="Z31" s="7"/>
     </row>
-    <row r="32" spans="2:26" s="50" customFormat="1">
+    <row r="32" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -6525,7 +6525,7 @@
       </c>
       <c r="Z32" s="7"/>
     </row>
-    <row r="33" spans="2:26" s="50" customFormat="1">
+    <row r="33" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -6559,8 +6559,8 @@
       </c>
       <c r="Z33" s="7"/>
     </row>
-    <row r="34" spans="2:26" s="50" customFormat="1"/>
-    <row r="35" spans="2:26" s="50" customFormat="1">
+    <row r="34" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -6594,7 +6594,7 @@
       </c>
       <c r="Z35" s="7"/>
     </row>
-    <row r="36" spans="2:26" s="50" customFormat="1">
+    <row r="36" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -6660,7 +6660,7 @@
       </c>
       <c r="Z36" s="7"/>
     </row>
-    <row r="37" spans="2:26" s="50" customFormat="1">
+    <row r="37" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -6694,7 +6694,7 @@
       </c>
       <c r="Z37" s="7"/>
     </row>
-    <row r="38" spans="2:26" s="50" customFormat="1"/>
+    <row r="38" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6714,19 +6714,19 @@
       <selection activeCell="Z37" sqref="Z37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="16" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="16" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="8" customWidth="1"/>
-    <col min="26" max="27" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D2" s="3">
         <v>2000</v>
       </c>
@@ -6794,7 +6794,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -6834,7 +6834,7 @@
       </c>
       <c r="Z3" s="5"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -6874,7 +6874,7 @@
       </c>
       <c r="Z4" s="5"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -6914,7 +6914,7 @@
       </c>
       <c r="Z5" s="5"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6948,7 +6948,7 @@
       </c>
       <c r="Z7" s="5"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6984,7 +6984,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -7018,7 +7018,7 @@
       </c>
       <c r="Z9" s="5"/>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7054,7 +7054,7 @@
       </c>
       <c r="Z11" s="5"/>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7096,7 +7096,7 @@
       </c>
       <c r="Z12" s="5"/>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7132,7 +7132,7 @@
       </c>
       <c r="Z13" s="5"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -7166,7 +7166,7 @@
       </c>
       <c r="Z15" s="5"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -7202,7 +7202,7 @@
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="17" spans="2:26">
+    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -7236,7 +7236,7 @@
       </c>
       <c r="Z17" s="5"/>
     </row>
-    <row r="19" spans="2:26">
+    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -7270,7 +7270,7 @@
       </c>
       <c r="Z19" s="5"/>
     </row>
-    <row r="20" spans="2:26">
+    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -7306,7 +7306,7 @@
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="21" spans="2:26">
+    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -7340,7 +7340,7 @@
       </c>
       <c r="Z21" s="5"/>
     </row>
-    <row r="23" spans="2:26">
+    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -7374,7 +7374,7 @@
       </c>
       <c r="Z23" s="5"/>
     </row>
-    <row r="24" spans="2:26">
+    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -7422,7 +7422,7 @@
       </c>
       <c r="Z24" s="5"/>
     </row>
-    <row r="25" spans="2:26">
+    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -7456,7 +7456,7 @@
       </c>
       <c r="Z25" s="5"/>
     </row>
-    <row r="27" spans="2:26">
+    <row r="27" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -7490,7 +7490,7 @@
       </c>
       <c r="Z27" s="5"/>
     </row>
-    <row r="28" spans="2:26">
+    <row r="28" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -7538,7 +7538,7 @@
       </c>
       <c r="Z28" s="5"/>
     </row>
-    <row r="29" spans="2:26">
+    <row r="29" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -7572,8 +7572,8 @@
       </c>
       <c r="Z29" s="5"/>
     </row>
-    <row r="30" spans="2:26" s="50" customFormat="1"/>
-    <row r="31" spans="2:26" s="50" customFormat="1">
+    <row r="30" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -7607,7 +7607,7 @@
       </c>
       <c r="Z31" s="5"/>
     </row>
-    <row r="32" spans="2:26" s="50" customFormat="1">
+    <row r="32" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -7646,7 +7646,7 @@
         <v>8.4000000000000003E-4</v>
       </c>
     </row>
-    <row r="33" spans="2:26" s="50" customFormat="1">
+    <row r="33" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -7680,8 +7680,8 @@
       </c>
       <c r="Z33" s="5"/>
     </row>
-    <row r="34" spans="2:26" s="50" customFormat="1"/>
-    <row r="35" spans="2:26" s="50" customFormat="1">
+    <row r="34" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -7715,7 +7715,7 @@
       </c>
       <c r="Z35" s="5"/>
     </row>
-    <row r="36" spans="2:26" s="50" customFormat="1">
+    <row r="36" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -7754,7 +7754,7 @@
         <v>1.2899999999999999E-3</v>
       </c>
     </row>
-    <row r="37" spans="2:26" s="50" customFormat="1">
+    <row r="37" spans="2:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -7807,14 +7807,14 @@
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C2" s="3">
         <v>2000</v>
       </c>
@@ -7882,7 +7882,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -7915,7 +7915,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -7948,7 +7948,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7981,7 +7981,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -8014,7 +8014,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -8047,7 +8047,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -8080,7 +8080,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -8113,7 +8113,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:25" s="50" customFormat="1">
+    <row r="10" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -8146,7 +8146,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:25" s="50" customFormat="1">
+    <row r="11" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -8179,12 +8179,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C16" s="3">
         <v>2000</v>
       </c>
@@ -8252,7 +8252,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -8285,7 +8285,7 @@
       </c>
       <c r="Y17" s="5"/>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -8318,7 +8318,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -8351,7 +8351,7 @@
       </c>
       <c r="Y19" s="5"/>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -8384,7 +8384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -8417,7 +8417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -8450,7 +8450,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -8483,7 +8483,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="24" spans="1:25" s="50" customFormat="1">
+    <row r="24" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -8516,7 +8516,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="25" spans="1:25" s="50" customFormat="1">
+    <row r="25" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -8549,12 +8549,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C30" s="3">
         <v>2000</v>
       </c>
@@ -8622,7 +8622,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -8655,7 +8655,7 @@
       </c>
       <c r="Y31" s="5"/>
     </row>
-    <row r="32" spans="1:25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -8688,7 +8688,7 @@
       </c>
       <c r="Y32" s="5"/>
     </row>
-    <row r="33" spans="2:25">
+    <row r="33" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -8721,7 +8721,7 @@
       </c>
       <c r="Y33" s="5"/>
     </row>
-    <row r="34" spans="2:25">
+    <row r="34" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -8754,7 +8754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:25">
+    <row r="35" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -8787,7 +8787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:25">
+    <row r="36" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -8820,7 +8820,7 @@
       </c>
       <c r="Y36" s="5"/>
     </row>
-    <row r="37" spans="2:25">
+    <row r="37" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -8853,7 +8853,7 @@
       </c>
       <c r="Y37" s="5"/>
     </row>
-    <row r="38" spans="2:25" s="50" customFormat="1">
+    <row r="38" spans="2:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -8886,7 +8886,7 @@
       </c>
       <c r="Y38" s="5"/>
     </row>
-    <row r="39" spans="2:25" s="50" customFormat="1">
+    <row r="39" spans="2:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -8938,14 +8938,14 @@
       <selection activeCell="Y54" sqref="Y54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C2" s="3">
         <v>2000</v>
       </c>
@@ -9013,7 +9013,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -9048,7 +9048,7 @@
       </c>
       <c r="Y3" s="9"/>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -9085,7 +9085,7 @@
       </c>
       <c r="Y4" s="9"/>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -9118,7 +9118,7 @@
       </c>
       <c r="Y5" s="9"/>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -9151,7 +9151,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -9184,7 +9184,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -9221,7 +9221,7 @@
       </c>
       <c r="Y8" s="9"/>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -9258,7 +9258,7 @@
       </c>
       <c r="Y9" s="9"/>
     </row>
-    <row r="10" spans="1:25" s="50" customFormat="1">
+    <row r="10" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -9291,7 +9291,7 @@
       </c>
       <c r="Y10" s="9"/>
     </row>
-    <row r="11" spans="1:25" s="50" customFormat="1">
+    <row r="11" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -9324,12 +9324,12 @@
       </c>
       <c r="Y11" s="9"/>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C16" s="3">
         <v>2000</v>
       </c>
@@ -9397,7 +9397,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>36</v>
       </c>
@@ -9429,12 +9429,12 @@
       </c>
       <c r="Y17" s="4"/>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="34" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C22" s="3">
         <v>2000</v>
       </c>
@@ -9502,7 +9502,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>25</v>
       </c>
@@ -9550,12 +9550,12 @@
       </c>
       <c r="Y23" s="4"/>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C29" s="3">
         <v>2000</v>
       </c>
@@ -9623,7 +9623,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -9656,7 +9656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -9689,7 +9689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -9722,7 +9722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -9755,7 +9755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -9788,7 +9788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -9821,7 +9821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -9854,7 +9854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:25" s="50" customFormat="1">
+    <row r="37" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -9887,7 +9887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:25" s="50" customFormat="1">
+    <row r="38" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -9920,12 +9920,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C43" s="3">
         <v>2000</v>
       </c>
@@ -9993,7 +9993,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
         <v>25</v>
       </c>
@@ -10027,12 +10027,12 @@
       </c>
       <c r="Y44" s="4"/>
     </row>
-    <row r="48" spans="1:25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C49" s="3">
         <v>2000</v>
       </c>
@@ -10100,7 +10100,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -10153,7 +10153,7 @@
       </c>
       <c r="Y50" s="8"/>
     </row>
-    <row r="51" spans="1:25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -10186,7 +10186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -10239,7 +10239,7 @@
       </c>
       <c r="Y52" s="8"/>
     </row>
-    <row r="53" spans="1:25" s="50" customFormat="1">
+    <row r="53" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -10272,12 +10272,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C58" s="3">
         <v>2000</v>
       </c>
@@ -10345,7 +10345,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
         <v>25</v>
       </c>
@@ -10396,20 +10396,20 @@
       <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C2" s="3">
         <v>2000</v>
       </c>
@@ -10477,7 +10477,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>25</v>
       </c>
@@ -10521,12 +10521,12 @@
       </c>
       <c r="Y3" s="8"/>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C8" s="3">
         <v>2000</v>
       </c>
@@ -10594,7 +10594,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
@@ -10628,12 +10628,12 @@
       </c>
       <c r="Y9" s="8"/>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C14" s="3">
         <v>2000</v>
       </c>
@@ -10701,7 +10701,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>25</v>
       </c>
@@ -10759,12 +10759,12 @@
       </c>
       <c r="Y15" s="8"/>
     </row>
-    <row r="19" spans="1:35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C20" s="3">
         <v>2000</v>
       </c>
@@ -10832,7 +10832,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>25</v>
       </c>
@@ -10890,7 +10890,7 @@
       </c>
       <c r="Y21" s="40"/>
     </row>
-    <row r="25" spans="1:35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
         <v>98</v>
       </c>
@@ -10929,7 +10929,7 @@
       <c r="AH25" s="29"/>
       <c r="AI25" s="29"/>
     </row>
-    <row r="26" spans="1:35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" s="29"/>
       <c r="B26" s="29"/>
       <c r="C26" s="31">
@@ -11030,7 +11030,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" s="29"/>
       <c r="B27" s="31" t="s">
         <v>25</v>
@@ -11071,12 +11071,12 @@
       </c>
       <c r="AI27" s="32"/>
     </row>
-    <row r="30" spans="1:35">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C31" s="3">
         <v>2000</v>
       </c>
@@ -11144,7 +11144,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:35">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>25</v>
       </c>
@@ -11202,12 +11202,12 @@
       </c>
       <c r="Y32" s="8"/>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C37" s="3">
         <v>2000</v>
       </c>
@@ -11275,7 +11275,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>25</v>
       </c>
@@ -11313,12 +11313,12 @@
       </c>
       <c r="Y38" s="8"/>
     </row>
-    <row r="39" spans="1:25" s="50" customFormat="1" ht="15" customHeight="1"/>
-    <row r="40" spans="1:25" s="50" customFormat="1" ht="15" customHeight="1"/>
-    <row r="41" spans="1:25" s="50" customFormat="1" ht="15" customHeight="1"/>
-    <row r="42" spans="1:25" s="50" customFormat="1">
+    <row r="39" spans="1:25" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:25" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:25" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="66" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B42" s="59"/>
       <c r="C42" s="59"/>
@@ -11345,7 +11345,7 @@
       <c r="X42" s="59"/>
       <c r="Y42" s="59"/>
     </row>
-    <row r="43" spans="1:25" s="50" customFormat="1">
+    <row r="43" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="59"/>
       <c r="B43" s="59"/>
       <c r="C43" s="67">
@@ -11416,7 +11416,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:25" s="50" customFormat="1">
+    <row r="44" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="59"/>
       <c r="B44" s="67" t="s">
         <v>36</v>
@@ -11447,12 +11447,12 @@
       </c>
       <c r="Y44" s="63"/>
     </row>
-    <row r="45" spans="1:25" s="50" customFormat="1"/>
-    <row r="46" spans="1:25" s="50" customFormat="1"/>
-    <row r="47" spans="1:25" s="50" customFormat="1"/>
-    <row r="48" spans="1:25" s="50" customFormat="1">
+    <row r="45" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="74" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B48" s="70"/>
       <c r="C48" s="70"/>
@@ -11479,7 +11479,7 @@
       <c r="X48" s="70"/>
       <c r="Y48" s="70"/>
     </row>
-    <row r="49" spans="1:25" s="50" customFormat="1">
+    <row r="49" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="70"/>
       <c r="B49" s="70"/>
       <c r="C49" s="71">
@@ -11550,7 +11550,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:25" s="50" customFormat="1">
+    <row r="50" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="70"/>
       <c r="B50" s="71" t="s">
         <v>36</v>
@@ -11581,7 +11581,7 @@
       </c>
       <c r="Y50" s="73"/>
     </row>
-    <row r="51" spans="1:25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A51" s="69"/>
       <c r="B51" s="69"/>
       <c r="C51" s="69"/>
@@ -11608,7 +11608,7 @@
       <c r="X51" s="69"/>
       <c r="Y51" s="69"/>
     </row>
-    <row r="52" spans="1:25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A52" s="69"/>
       <c r="B52" s="69"/>
       <c r="C52" s="69"/>
@@ -11635,7 +11635,7 @@
       <c r="X52" s="69"/>
       <c r="Y52" s="69"/>
     </row>
-    <row r="53" spans="1:25">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A53" s="69"/>
       <c r="B53" s="69"/>
       <c r="C53" s="69"/>
@@ -11662,9 +11662,9 @@
       <c r="X53" s="69"/>
       <c r="Y53" s="69"/>
     </row>
-    <row r="54" spans="1:25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" s="74" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B54" s="70"/>
       <c r="C54" s="70"/>
@@ -11691,7 +11691,7 @@
       <c r="X54" s="70"/>
       <c r="Y54" s="70"/>
     </row>
-    <row r="55" spans="1:25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" s="70"/>
       <c r="B55" s="70"/>
       <c r="C55" s="71">
@@ -11762,7 +11762,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" s="70"/>
       <c r="B56" s="71" t="s">
         <v>36</v>
@@ -11811,9 +11811,9 @@
       <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="58" t="s">
         <v>108</v>
       </c>
@@ -11842,7 +11842,7 @@
       <c r="X1" s="50"/>
       <c r="Y1" s="50"/>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="57"/>
       <c r="B2" s="50"/>
       <c r="C2" s="52">
@@ -11913,7 +11913,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="57"/>
       <c r="B3" s="3" t="str">
         <f>Populations!$C$3</f>
@@ -11947,7 +11947,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="57"/>
       <c r="B4" s="3" t="str">
         <f>Populations!$C$4</f>
@@ -11981,7 +11981,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="50"/>
       <c r="B5" s="3" t="str">
         <f>Populations!$C$5</f>
@@ -12015,7 +12015,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="50"/>
       <c r="B6" s="3" t="str">
         <f>Populations!$C$6</f>
@@ -12049,7 +12049,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="50"/>
       <c r="B7" s="3" t="str">
         <f>Populations!$C$7</f>
@@ -12083,7 +12083,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -12116,7 +12116,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="57"/>
       <c r="B9" s="3" t="str">
         <f>Populations!$C$9</f>
@@ -12150,7 +12150,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:25" s="50" customFormat="1">
+    <row r="10" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="57"/>
       <c r="B10" s="3" t="str">
         <f>Populations!$C$10</f>
@@ -12184,7 +12184,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:25" s="50" customFormat="1">
+    <row r="11" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="57"/>
       <c r="B11" s="3" t="str">
         <f>Populations!$C$11</f>
@@ -12218,9 +12218,9 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="58" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B15" s="50"/>
       <c r="C15" s="50"/>
@@ -12247,7 +12247,7 @@
       <c r="X15" s="50"/>
       <c r="Y15" s="50"/>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="57"/>
       <c r="B16" s="50"/>
       <c r="C16" s="52">
@@ -12318,7 +12318,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -12351,7 +12351,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="57"/>
       <c r="B18" s="3" t="str">
         <f>Populations!$C$4</f>
@@ -12385,7 +12385,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="50"/>
       <c r="B19" s="3" t="str">
         <f>Populations!$C$5</f>
@@ -12419,7 +12419,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="50"/>
       <c r="B20" s="3" t="str">
         <f>Populations!$C$6</f>
@@ -12453,7 +12453,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="50"/>
       <c r="B21" s="3" t="str">
         <f>Populations!$C$7</f>
@@ -12487,7 +12487,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -12520,7 +12520,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="50"/>
       <c r="B23" s="3" t="str">
         <f>Populations!$C$9</f>
@@ -12554,7 +12554,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="24" spans="1:25" s="50" customFormat="1">
+    <row r="24" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -12587,7 +12587,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="25" spans="1:25" s="50" customFormat="1">
+    <row r="25" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -12620,7 +12620,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="58" t="s">
         <v>109</v>
       </c>
@@ -12649,7 +12649,7 @@
       <c r="X29" s="50"/>
       <c r="Y29" s="50"/>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="50"/>
       <c r="B30" s="50"/>
       <c r="C30" s="52">
@@ -12720,7 +12720,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="50"/>
       <c r="B31" s="3" t="str">
         <f>Populations!$C$3</f>
@@ -12754,7 +12754,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="32" spans="1:25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="50"/>
       <c r="B32" s="3" t="str">
         <f>Populations!$C$4</f>
@@ -12788,7 +12788,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="33" spans="1:25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="50"/>
       <c r="B33" s="3" t="str">
         <f>Populations!$C$5</f>
@@ -12822,7 +12822,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="34" spans="1:25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="50"/>
       <c r="B34" s="3" t="str">
         <f>Populations!$C$6</f>
@@ -12856,7 +12856,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="35" spans="1:25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="50"/>
       <c r="B35" s="3" t="str">
         <f>Populations!$C$7</f>
@@ -12890,7 +12890,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="50"/>
       <c r="B36" s="3" t="str">
         <f>Populations!$C$8</f>
@@ -12924,7 +12924,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="50"/>
       <c r="B37" s="3" t="str">
         <f>Populations!$C$9</f>
@@ -12958,7 +12958,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="38" spans="1:25" s="50" customFormat="1">
+    <row r="38" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -12991,7 +12991,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="39" spans="1:25" s="50" customFormat="1">
+    <row r="39" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -13024,7 +13024,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="43" spans="1:25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="58" t="s">
         <v>110</v>
       </c>
@@ -13053,7 +13053,7 @@
       <c r="X43" s="50"/>
       <c r="Y43" s="50"/>
     </row>
-    <row r="44" spans="1:25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="50"/>
       <c r="B44" s="50"/>
       <c r="C44" s="52">
@@ -13124,7 +13124,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="50"/>
       <c r="B45" s="3" t="str">
         <f>Populations!$C$3</f>
@@ -13158,7 +13158,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="46" spans="1:25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="50"/>
       <c r="B46" s="3" t="str">
         <f>Populations!$C$4</f>
@@ -13192,7 +13192,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="47" spans="1:25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" s="50"/>
       <c r="B47" s="3" t="str">
         <f>Populations!$C$5</f>
@@ -13226,7 +13226,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="48" spans="1:25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" s="50"/>
       <c r="B48" s="3" t="str">
         <f>Populations!$C$6</f>
@@ -13260,7 +13260,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="49" spans="1:25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49" s="50"/>
       <c r="B49" s="3" t="str">
         <f>Populations!$C$7</f>
@@ -13294,7 +13294,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="50" spans="1:25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A50" s="50"/>
       <c r="B50" s="3" t="str">
         <f>Populations!$C$8</f>
@@ -13328,7 +13328,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="51" spans="1:25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A51" s="50"/>
       <c r="B51" s="3" t="str">
         <f>Populations!$C$9</f>
@@ -13362,7 +13362,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="52" spans="1:25" s="50" customFormat="1">
+    <row r="52" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -13395,7 +13395,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="53" spans="1:25" s="50" customFormat="1">
+    <row r="53" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -13428,9 +13428,9 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="57" spans="1:25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57" s="60" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B57" s="59"/>
       <c r="C57" s="59"/>
@@ -13457,7 +13457,7 @@
       <c r="X57" s="59"/>
       <c r="Y57" s="59"/>
     </row>
-    <row r="58" spans="1:25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A58" s="59"/>
       <c r="B58" s="59"/>
       <c r="C58" s="61">
@@ -13528,7 +13528,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A59" s="59"/>
       <c r="B59" s="61" t="s">
         <v>36</v>
@@ -13561,7 +13561,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="63" spans="1:25">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A63" s="60" t="s">
         <v>107</v>
       </c>
@@ -13590,7 +13590,7 @@
       <c r="X63" s="59"/>
       <c r="Y63" s="59"/>
     </row>
-    <row r="64" spans="1:25">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A64" s="59"/>
       <c r="B64" s="59"/>
       <c r="C64" s="61">
@@ -13661,7 +13661,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65" s="59"/>
       <c r="B65" s="61" t="s">
         <v>36</v>
@@ -13694,9 +13694,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="69" spans="1:25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" s="60" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B69" s="59"/>
       <c r="C69" s="59"/>
@@ -13723,7 +13723,7 @@
       <c r="X69" s="59"/>
       <c r="Y69" s="59"/>
     </row>
-    <row r="70" spans="1:25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" s="59"/>
       <c r="B70" s="59"/>
       <c r="C70" s="61">
@@ -13794,7 +13794,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" s="59"/>
       <c r="B71" s="61" t="s">
         <v>36</v>
@@ -13827,9 +13827,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" s="60" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B75" s="59"/>
       <c r="C75" s="59"/>
@@ -13856,7 +13856,7 @@
       <c r="X75" s="59"/>
       <c r="Y75" s="59"/>
     </row>
-    <row r="76" spans="1:25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" s="59"/>
       <c r="B76" s="59"/>
       <c r="C76" s="61">
@@ -13927,7 +13927,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A77" s="59"/>
       <c r="B77" s="61" t="s">
         <v>36</v>
@@ -13960,9 +13960,9 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="81" spans="1:25">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A81" s="60" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B81" s="59"/>
       <c r="C81" s="59"/>
@@ -13989,7 +13989,7 @@
       <c r="X81" s="59"/>
       <c r="Y81" s="59"/>
     </row>
-    <row r="82" spans="1:25">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A82" s="59"/>
       <c r="B82" s="59"/>
       <c r="C82" s="61">
@@ -14060,7 +14060,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="83" spans="1:25">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A83" s="59"/>
       <c r="B83" s="61" t="s">
         <v>36</v>
@@ -14093,9 +14093,9 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="87" spans="1:25">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A87" s="60" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B87" s="59"/>
       <c r="C87" s="59"/>
@@ -14122,7 +14122,7 @@
       <c r="X87" s="59"/>
       <c r="Y87" s="59"/>
     </row>
-    <row r="88" spans="1:25">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A88" s="59"/>
       <c r="B88" s="59"/>
       <c r="C88" s="61">
@@ -14193,7 +14193,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="89" spans="1:25">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A89" s="59"/>
       <c r="B89" s="61" t="s">
         <v>36</v>
@@ -14241,18 +14241,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C72" workbookViewId="0">
-      <selection activeCell="M91" sqref="M91"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C2" s="3">
         <v>2000</v>
       </c>
@@ -14320,7 +14318,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -14353,7 +14351,7 @@
       </c>
       <c r="Y3" s="4"/>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -14386,7 +14384,7 @@
       </c>
       <c r="Y4" s="4"/>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -14419,7 +14417,7 @@
       </c>
       <c r="Y5" s="4"/>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -14452,7 +14450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -14485,7 +14483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -14518,7 +14516,7 @@
       </c>
       <c r="Y8" s="4"/>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -14551,7 +14549,7 @@
       </c>
       <c r="Y9" s="4"/>
     </row>
-    <row r="10" spans="1:25" s="50" customFormat="1">
+    <row r="10" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -14584,7 +14582,7 @@
       </c>
       <c r="Y10" s="4"/>
     </row>
-    <row r="11" spans="1:25" s="50" customFormat="1">
+    <row r="11" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -14617,12 +14615,12 @@
       </c>
       <c r="Y11" s="4"/>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C16" s="3">
         <v>2000</v>
       </c>
@@ -14690,7 +14688,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -14723,7 +14721,7 @@
       </c>
       <c r="Y17" s="4"/>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -14756,7 +14754,7 @@
       </c>
       <c r="Y18" s="4"/>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -14789,7 +14787,7 @@
       </c>
       <c r="Y19" s="4"/>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -14822,7 +14820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -14855,7 +14853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -14888,7 +14886,7 @@
       </c>
       <c r="Y22" s="4"/>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -14921,7 +14919,7 @@
       </c>
       <c r="Y23" s="4"/>
     </row>
-    <row r="24" spans="1:25" s="50" customFormat="1">
+    <row r="24" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -14954,7 +14952,7 @@
       </c>
       <c r="Y24" s="4"/>
     </row>
-    <row r="25" spans="1:25" s="50" customFormat="1">
+    <row r="25" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -14987,12 +14985,12 @@
       </c>
       <c r="Y25" s="4"/>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C30" s="3">
         <v>2000</v>
       </c>
@@ -15060,7 +15058,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -15093,7 +15091,7 @@
       </c>
       <c r="Y31" s="4"/>
     </row>
-    <row r="32" spans="1:25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -15126,7 +15124,7 @@
       </c>
       <c r="Y32" s="4"/>
     </row>
-    <row r="33" spans="1:25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -15159,7 +15157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -15192,7 +15190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -15225,7 +15223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -15258,7 +15256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -15291,7 +15289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:25" s="50" customFormat="1">
+    <row r="38" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -15324,7 +15322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:25" s="50" customFormat="1">
+    <row r="39" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -15357,12 +15355,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C44" s="3">
         <v>2000</v>
       </c>
@@ -15430,7 +15428,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -15463,7 +15461,7 @@
       </c>
       <c r="Y45" s="9"/>
     </row>
-    <row r="46" spans="1:25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -15496,7 +15494,7 @@
       </c>
       <c r="Y46" s="9"/>
     </row>
-    <row r="47" spans="1:25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -15529,7 +15527,7 @@
       </c>
       <c r="Y47" s="9"/>
     </row>
-    <row r="48" spans="1:25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -15562,7 +15560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -15595,7 +15593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -15628,7 +15626,7 @@
       </c>
       <c r="Y50" s="9"/>
     </row>
-    <row r="51" spans="1:25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -15661,7 +15659,7 @@
       </c>
       <c r="Y51" s="9"/>
     </row>
-    <row r="52" spans="1:25" s="50" customFormat="1">
+    <row r="52" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -15694,7 +15692,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:25" s="50" customFormat="1">
+    <row r="53" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -15727,12 +15725,12 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="1:25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C58" s="3">
         <v>2000</v>
       </c>
@@ -15800,7 +15798,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -15833,7 +15831,7 @@
       </c>
       <c r="Y59" s="9"/>
     </row>
-    <row r="60" spans="1:25">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -15870,7 +15868,7 @@
       </c>
       <c r="Y60" s="9"/>
     </row>
-    <row r="61" spans="1:25">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -15903,7 +15901,7 @@
       </c>
       <c r="Y61" s="9"/>
     </row>
-    <row r="62" spans="1:25">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -15936,7 +15934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:25">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -15969,7 +15967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:25">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -16006,7 +16004,7 @@
       </c>
       <c r="Y64" s="9"/>
     </row>
-    <row r="65" spans="1:25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -16043,7 +16041,7 @@
       </c>
       <c r="Y65" s="9"/>
     </row>
-    <row r="66" spans="1:25" s="50" customFormat="1">
+    <row r="66" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -16076,7 +16074,7 @@
       </c>
       <c r="Y66" s="9"/>
     </row>
-    <row r="67" spans="1:25" s="50" customFormat="1">
+    <row r="67" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -16109,12 +16107,12 @@
       </c>
       <c r="Y67" s="9"/>
     </row>
-    <row r="71" spans="1:25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="72" spans="1:25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C72" s="3">
         <v>2000</v>
       </c>
@@ -16182,7 +16180,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -16217,7 +16215,7 @@
       </c>
       <c r="Y73" s="9"/>
     </row>
-    <row r="74" spans="1:25">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -16250,7 +16248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -16283,7 +16281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -16316,7 +16314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B77" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -16349,7 +16347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:25">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -16382,7 +16380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -16415,7 +16413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:25" s="50" customFormat="1">
+    <row r="80" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -16448,7 +16446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:25" s="50" customFormat="1">
+    <row r="81" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -16481,12 +16479,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:25">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="86" spans="1:25">
+    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C86" s="3">
         <v>2000</v>
       </c>
@@ -16554,7 +16552,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="87" spans="1:25">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -16587,7 +16585,7 @@
       </c>
       <c r="Y87" s="9"/>
     </row>
-    <row r="88" spans="1:25">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B88" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -16620,7 +16618,7 @@
       </c>
       <c r="Y88" s="9"/>
     </row>
-    <row r="89" spans="1:25">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B89" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -16653,7 +16651,7 @@
       </c>
       <c r="Y89" s="9"/>
     </row>
-    <row r="90" spans="1:25">
+    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B90" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -16686,7 +16684,7 @@
       </c>
       <c r="Y90" s="9"/>
     </row>
-    <row r="91" spans="1:25" s="50" customFormat="1">
+    <row r="91" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>

</xml_diff>

<commit_message>
working, but circumcision still not intervenable
</commit_message>
<xml_diff>
--- a/tests/generalized.xlsx
+++ b/tests/generalized.xlsx
@@ -477,6 +477,9 @@
     <t>F 50+</t>
   </si>
   <si>
+    <t>Males 15-49</t>
+  </si>
+  <si>
     <t>Females 15-49</t>
   </si>
   <si>
@@ -514,9 +517,6 @@
   </si>
   <si>
     <t>PLHIV in care on treatment (%)</t>
-  </si>
-  <si>
-    <t>Males 15-49kk</t>
   </si>
 </sst>
 </file>
@@ -3646,7 +3646,7 @@
     <row r="65" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="66" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="67" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
@@ -5140,7 +5140,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5335,7 +5335,7 @@
         <v>117</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>9</v>
@@ -5364,7 +5364,7 @@
         <v>118</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>8</v>
@@ -5393,7 +5393,7 @@
         <v>119</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>9</v>
@@ -5422,7 +5422,7 @@
         <v>120</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>8</v>
@@ -11318,7 +11318,7 @@
     <row r="41" spans="1:25" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="66" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B42" s="59"/>
       <c r="C42" s="59"/>
@@ -11452,7 +11452,7 @@
     <row r="47" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="1:25" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="74" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B48" s="70"/>
       <c r="C48" s="70"/>
@@ -11664,7 +11664,7 @@
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" s="74" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B54" s="70"/>
       <c r="C54" s="70"/>
@@ -12220,7 +12220,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="58" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B15" s="50"/>
       <c r="C15" s="50"/>
@@ -13430,7 +13430,7 @@
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57" s="60" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B57" s="59"/>
       <c r="C57" s="59"/>
@@ -13696,7 +13696,7 @@
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" s="60" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B69" s="59"/>
       <c r="C69" s="59"/>
@@ -13829,7 +13829,7 @@
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" s="60" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B75" s="59"/>
       <c r="C75" s="59"/>
@@ -13962,7 +13962,7 @@
     </row>
     <row r="81" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A81" s="60" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B81" s="59"/>
       <c r="C81" s="59"/>
@@ -14095,7 +14095,7 @@
     </row>
     <row r="87" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A87" s="60" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B87" s="59"/>
       <c r="C87" s="59"/>

</xml_diff>

<commit_message>
now testing rates actually increase
</commit_message>
<xml_diff>
--- a/tests/generalized.xlsx
+++ b/tests/generalized.xlsx
@@ -8250,8 +8250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8380,17 +8380,17 @@
       <c r="H4" s="19"/>
       <c r="I4" s="19"/>
       <c r="J4" s="19">
-        <v>0.2215</v>
+        <v>0.122</v>
       </c>
       <c r="K4" s="19"/>
       <c r="L4" s="19">
-        <v>0.35849999999999999</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="M4" s="19"/>
       <c r="N4" s="20"/>
       <c r="O4" s="20"/>
       <c r="P4" s="20">
-        <v>0.42599999999999999</v>
+        <v>0.184</v>
       </c>
       <c r="Q4" s="20"/>
       <c r="R4" s="20"/>
@@ -8516,17 +8516,17 @@
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
       <c r="J8" s="19">
-        <v>0.23200000000000001</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="K8" s="19"/>
       <c r="L8" s="19">
-        <v>0.38650000000000001</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="M8" s="19"/>
       <c r="N8" s="20"/>
       <c r="O8" s="19"/>
       <c r="P8" s="20">
-        <v>0.46350000000000002</v>
+        <v>0.113</v>
       </c>
       <c r="Q8" s="20"/>
       <c r="R8" s="20"/>
@@ -8553,17 +8553,17 @@
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
       <c r="J9" s="19">
-        <v>0.22900000000000001</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="K9" s="19"/>
       <c r="L9" s="19">
-        <v>0.38250000000000001</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="M9" s="19"/>
       <c r="N9" s="20"/>
       <c r="O9" s="19"/>
       <c r="P9" s="20">
-        <v>0.46250000000000002</v>
+        <v>0.113</v>
       </c>
       <c r="Q9" s="20"/>
       <c r="R9" s="20"/>
@@ -8596,7 +8596,7 @@
       <c r="N10" s="20"/>
       <c r="O10" s="19"/>
       <c r="P10" s="20">
-        <v>0.3</v>
+        <v>0.06</v>
       </c>
       <c r="Q10" s="20"/>
       <c r="R10" s="20"/>
@@ -8629,7 +8629,7 @@
       <c r="N11" s="20"/>
       <c r="O11" s="19"/>
       <c r="P11" s="20">
-        <v>0.3</v>
+        <v>0.06</v>
       </c>
       <c r="Q11" s="20"/>
       <c r="R11" s="20"/>
@@ -13157,8 +13157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y101"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P68" sqref="P68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14731,7 +14731,7 @@
       <c r="J59" s="20"/>
       <c r="K59" s="20"/>
       <c r="L59" s="44">
-        <v>0.378</v>
+        <v>0.21299999999999999</v>
       </c>
       <c r="M59" s="44"/>
       <c r="N59" s="20"/>
@@ -14766,13 +14766,13 @@
       </c>
       <c r="K60" s="20"/>
       <c r="L60" s="26">
-        <v>0.39</v>
+        <v>0.21299999999999999</v>
       </c>
       <c r="M60" s="26"/>
       <c r="N60" s="20"/>
       <c r="O60" s="20"/>
       <c r="P60" s="20">
-        <v>0.51249999999999996</v>
+        <v>0.28299999999999997</v>
       </c>
       <c r="Q60" s="20"/>
       <c r="R60" s="20"/>
@@ -14902,13 +14902,13 @@
       </c>
       <c r="K64" s="20"/>
       <c r="L64" s="20">
-        <v>0.4</v>
+        <v>0.15</v>
       </c>
       <c r="M64" s="20"/>
       <c r="N64" s="20"/>
       <c r="O64" s="20"/>
       <c r="P64" s="20">
-        <v>0.53749999999999998</v>
+        <v>0.18</v>
       </c>
       <c r="Q64" s="20"/>
       <c r="R64" s="20"/>
@@ -14939,13 +14939,13 @@
       </c>
       <c r="K65" s="20"/>
       <c r="L65" s="26">
-        <v>0.39500000000000002</v>
+        <v>0.15</v>
       </c>
       <c r="M65" s="26"/>
       <c r="N65" s="20"/>
       <c r="O65" s="20"/>
       <c r="P65" s="20">
-        <v>0.53500000000000003</v>
+        <v>0.18</v>
       </c>
       <c r="Q65" s="20"/>
       <c r="R65" s="20"/>
@@ -14978,7 +14978,7 @@
       <c r="N66" s="20"/>
       <c r="O66" s="20"/>
       <c r="P66" s="20">
-        <v>0.3</v>
+        <v>0.22</v>
       </c>
       <c r="Q66" s="20"/>
       <c r="R66" s="20"/>
@@ -15011,7 +15011,7 @@
       <c r="N67" s="20"/>
       <c r="O67" s="20"/>
       <c r="P67" s="20">
-        <v>0.3</v>
+        <v>0.22</v>
       </c>
       <c r="Q67" s="20"/>
       <c r="R67" s="20"/>

</xml_diff>

<commit_message>
write largely pointless migration
</commit_message>
<xml_diff>
--- a/tests/generalized.xlsx
+++ b/tests/generalized.xlsx
@@ -691,7 +691,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="122">
+  <cellStyleXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
@@ -806,6 +806,8 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -953,7 +955,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="122">
+  <cellStyles count="124">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="6"/>
     <cellStyle name="Comma 2 2" xfId="14"/>
@@ -964,6 +966,7 @@
     <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink 10" xfId="25"/>
     <cellStyle name="Followed Hyperlink 11" xfId="26"/>
     <cellStyle name="Followed Hyperlink 12" xfId="27"/>
@@ -1065,6 +1068,7 @@
     <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="4"/>
     <cellStyle name="Normal 2 2" xfId="15"/>
@@ -12078,7 +12082,7 @@
   <dimension ref="A1:Y57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3:Y11"/>
+      <selection activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -12188,7 +12192,7 @@
         <v>35</v>
       </c>
       <c r="Y3" s="53">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -12222,7 +12226,7 @@
         <v>35</v>
       </c>
       <c r="Y4" s="53">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="5" spans="1:25">

</xml_diff>

<commit_message>
just have to do migrations now
</commit_message>
<xml_diff>
--- a/tests/generalized.xlsx
+++ b/tests/generalized.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/optima/tests/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24220" windowHeight="12800" tabRatio="988" firstSheet="2" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24220" windowHeight="12800" tabRatio="988" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -20,8 +25,11 @@
     <sheet name="Partnerships &amp; transitions" sheetId="11" r:id="rId11"/>
     <sheet name="Constants" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -1020,12 +1028,12 @@
     <xf numFmtId="171" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="4" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="149">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1980,55 +1988,55 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="80.6640625" customWidth="1"/>
+    <col min="1" max="1" width="80.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="72" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="69"/>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="69"/>
-    </row>
-    <row r="4" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="72"/>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="72"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="66"/>
     </row>
-    <row r="5" spans="1:1" ht="42">
+    <row r="5" spans="1:1" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="66" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="66"/>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="66" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="66"/>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="66" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="66"/>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="66" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="66"/>
     </row>
   </sheetData>
@@ -2037,11 +2045,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2053,14 +2056,14 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C2" s="4">
         <v>2000</v>
       </c>
@@ -2128,7 +2131,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2161,7 +2164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2194,7 +2197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2227,7 +2230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -2260,7 +2263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -2293,7 +2296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -2326,7 +2329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -2359,7 +2362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -2392,7 +2395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -2425,12 +2428,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C16" s="4">
         <v>2000</v>
       </c>
@@ -2498,7 +2501,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2531,7 +2534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2564,7 +2567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2597,7 +2600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -2630,7 +2633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B21" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -2663,7 +2666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B22" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -2696,7 +2699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -2729,7 +2732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B24" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -2762,7 +2765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B25" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -2795,12 +2798,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C30" s="4">
         <v>2000</v>
       </c>
@@ -2868,7 +2871,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B31" s="4" t="s">
         <v>40</v>
       </c>
@@ -2903,11 +2906,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2919,14 +2917,14 @@
       <selection activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C2" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2964,7 +2962,7 @@
         <v>F 50+</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2979,7 +2977,7 @@
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3000,7 +2998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3017,7 +3015,7 @@
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -3032,7 +3030,7 @@
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -3047,7 +3045,7 @@
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -3068,7 +3066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -3083,7 +3081,7 @@
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -3104,7 +3102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -3119,12 +3117,12 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C16" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3162,7 +3160,7 @@
         <v>F 50+</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3177,7 +3175,7 @@
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3198,7 +3196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3215,7 +3213,7 @@
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -3230,7 +3228,7 @@
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B21" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -3245,7 +3243,7 @@
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B22" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -3266,7 +3264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -3281,7 +3279,7 @@
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B24" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -3302,7 +3300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B25" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -3317,12 +3315,12 @@
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C30" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3360,7 +3358,7 @@
         <v>F 50+</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B31" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3375,7 +3373,7 @@
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B32" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3392,7 +3390,7 @@
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B33" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3407,7 +3405,7 @@
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B34" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -3422,7 +3420,7 @@
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B35" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -3437,7 +3435,7 @@
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B36" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -3452,7 +3450,7 @@
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B37" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -3467,7 +3465,7 @@
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B38" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -3482,7 +3480,7 @@
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B39" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -3497,12 +3495,12 @@
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C44" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3540,7 +3538,7 @@
         <v>F 50+</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3555,7 +3553,7 @@
       <c r="J45" s="5"/>
       <c r="K45" s="5"/>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B46" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3570,7 +3568,7 @@
       <c r="J46" s="5"/>
       <c r="K46" s="5"/>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B47" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3585,7 +3583,7 @@
       <c r="J47" s="5"/>
       <c r="K47" s="5"/>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B48" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -3600,7 +3598,7 @@
       <c r="J48" s="5"/>
       <c r="K48" s="5"/>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B49" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -3615,7 +3613,7 @@
       <c r="J49" s="5"/>
       <c r="K49" s="5"/>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B50" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -3630,7 +3628,7 @@
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B51" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -3645,7 +3643,7 @@
       <c r="J51" s="5"/>
       <c r="K51" s="5"/>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B52" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -3660,7 +3658,7 @@
       <c r="J52" s="5"/>
       <c r="K52" s="5"/>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B53" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -3675,12 +3673,12 @@
       <c r="J53" s="5"/>
       <c r="K53" s="5"/>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C58" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3718,7 +3716,7 @@
         <v>F 50+</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B59" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3737,7 +3735,7 @@
       <c r="J59" s="5"/>
       <c r="K59" s="5"/>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B60" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -3752,7 +3750,7 @@
       <c r="J60" s="5"/>
       <c r="K60" s="5"/>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B61" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -3771,7 +3769,7 @@
       <c r="J61" s="5"/>
       <c r="K61" s="5"/>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B62" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -3786,12 +3784,12 @@
       <c r="J62" s="5"/>
       <c r="K62" s="5"/>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C67" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3829,7 +3827,7 @@
         <v>F 50+</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B68" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3844,7 +3842,7 @@
       <c r="J68" s="5"/>
       <c r="K68" s="5"/>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B69" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3859,7 +3857,7 @@
       <c r="J69" s="5"/>
       <c r="K69" s="5"/>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B70" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3874,7 +3872,7 @@
       <c r="J70" s="5"/>
       <c r="K70" s="5"/>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B71" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -3891,7 +3889,7 @@
       <c r="J71" s="5"/>
       <c r="K71" s="5"/>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B72" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -3908,7 +3906,7 @@
       <c r="J72" s="5"/>
       <c r="K72" s="5"/>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B73" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -3925,7 +3923,7 @@
       </c>
       <c r="K73" s="5"/>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B74" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -3942,7 +3940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B75" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -3957,7 +3955,7 @@
       <c r="J75" s="5"/>
       <c r="K75" s="5"/>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B76" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -3972,12 +3970,12 @@
       <c r="J76" s="5"/>
       <c r="K76" s="5"/>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="81" spans="2:11">
+    <row r="81" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C81" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -4015,7 +4013,7 @@
         <v>F 50+</v>
       </c>
     </row>
-    <row r="82" spans="2:11">
+    <row r="82" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B82" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -4034,7 +4032,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="2:11">
+    <row r="83" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B83" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -4053,7 +4051,7 @@
       </c>
       <c r="K83" s="5"/>
     </row>
-    <row r="84" spans="2:11">
+    <row r="84" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B84" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -4068,7 +4066,7 @@
       <c r="J84" s="5"/>
       <c r="K84" s="5"/>
     </row>
-    <row r="85" spans="2:11">
+    <row r="85" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B85" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -4083,7 +4081,7 @@
       <c r="J85" s="5"/>
       <c r="K85" s="5"/>
     </row>
-    <row r="86" spans="2:11">
+    <row r="86" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B86" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -4098,7 +4096,7 @@
       <c r="J86" s="5"/>
       <c r="K86" s="5"/>
     </row>
-    <row r="87" spans="2:11">
+    <row r="87" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B87" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -4113,7 +4111,7 @@
       <c r="J87" s="5"/>
       <c r="K87" s="5"/>
     </row>
-    <row r="88" spans="2:11">
+    <row r="88" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B88" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -4128,7 +4126,7 @@
       <c r="J88" s="5"/>
       <c r="K88" s="5"/>
     </row>
-    <row r="89" spans="2:11">
+    <row r="89" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B89" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -4143,7 +4141,7 @@
       <c r="J89" s="5"/>
       <c r="K89" s="5"/>
     </row>
-    <row r="90" spans="2:11">
+    <row r="90" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B90" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -4161,11 +4159,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4173,17 +4166,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A41" sqref="A41:XFD41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="37.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="44" t="s">
         <v>73</v>
       </c>
@@ -4192,7 +4185,7 @@
       <c r="D1" s="45"/>
       <c r="E1" s="45"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="45"/>
       <c r="B2" s="45"/>
       <c r="C2" s="46" t="s">
@@ -4205,7 +4198,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="45"/>
       <c r="B3" s="47" t="s">
         <v>74</v>
@@ -4220,7 +4213,7 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="45"/>
       <c r="B4" s="47" t="s">
         <v>75</v>
@@ -4235,7 +4228,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="45"/>
       <c r="B5" s="47" t="s">
         <v>76</v>
@@ -4250,7 +4243,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="45"/>
       <c r="B6" s="47" t="s">
         <v>77</v>
@@ -4265,7 +4258,7 @@
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="45"/>
       <c r="B7" s="47" t="s">
         <v>78</v>
@@ -4280,7 +4273,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="45"/>
       <c r="B8" s="47" t="s">
         <v>79</v>
@@ -4295,7 +4288,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="45"/>
       <c r="B9" s="47" t="s">
         <v>80</v>
@@ -4310,33 +4303,33 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="51"/>
       <c r="B10" s="52"/>
       <c r="C10" s="51"/>
       <c r="D10" s="51"/>
       <c r="E10" s="51"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="51"/>
       <c r="B11" s="52"/>
       <c r="C11" s="51"/>
       <c r="D11" s="51"/>
       <c r="E11" s="51"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="51"/>
       <c r="B12" s="52"/>
       <c r="C12" s="51"/>
       <c r="D12" s="51"/>
       <c r="E12" s="51"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C14" s="4" t="s">
         <v>32</v>
       </c>
@@ -4347,7 +4340,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>82</v>
       </c>
@@ -4361,7 +4354,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>83</v>
       </c>
@@ -4375,7 +4368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>84</v>
       </c>
@@ -4389,7 +4382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>85</v>
       </c>
@@ -4403,7 +4396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>86</v>
       </c>
@@ -4417,7 +4410,7 @@
         <v>6.92</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>87</v>
       </c>
@@ -4431,33 +4424,33 @@
         <v>12.08</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="51"/>
       <c r="B21" s="52"/>
       <c r="C21" s="51"/>
       <c r="D21" s="51"/>
       <c r="E21" s="51"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="51"/>
       <c r="B22" s="52"/>
       <c r="C22" s="51"/>
       <c r="D22" s="51"/>
       <c r="E22" s="51"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="51"/>
       <c r="B23" s="52"/>
       <c r="C23" s="51"/>
       <c r="D23" s="51"/>
       <c r="E23" s="51"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C25" s="4" t="s">
         <v>32</v>
       </c>
@@ -4468,7 +4461,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>88</v>
       </c>
@@ -4482,7 +4475,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>84</v>
       </c>
@@ -4497,7 +4490,7 @@
       </c>
       <c r="G27" s="53"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>89</v>
       </c>
@@ -4511,7 +4504,7 @@
         <v>3.16</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>90</v>
       </c>
@@ -4525,7 +4518,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>91</v>
       </c>
@@ -4539,33 +4532,33 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="51"/>
       <c r="B31" s="52"/>
       <c r="C31" s="51"/>
       <c r="D31" s="51"/>
       <c r="E31" s="51"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="51"/>
       <c r="B32" s="52"/>
       <c r="C32" s="51"/>
       <c r="D32" s="51"/>
       <c r="E32" s="51"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="51"/>
       <c r="B33" s="52"/>
       <c r="C33" s="51"/>
       <c r="D33" s="51"/>
       <c r="E33" s="51"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C35" s="4" t="s">
         <v>32</v>
       </c>
@@ -4576,7 +4569,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
         <v>92</v>
       </c>
@@ -4590,7 +4583,7 @@
         <v>7.28</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>93</v>
       </c>
@@ -4604,7 +4597,7 @@
         <v>3.42</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
         <v>94</v>
       </c>
@@ -4618,7 +4611,7 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>95</v>
       </c>
@@ -4632,7 +4625,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="42" customFormat="1">
+    <row r="40" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="40"/>
       <c r="B40" s="2" t="s">
         <v>119</v>
@@ -4647,46 +4640,46 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C41" s="70">
+      <c r="C41" s="69">
         <v>2</v>
       </c>
-      <c r="D41" s="71">
+      <c r="D41" s="70">
         <v>1.5</v>
       </c>
-      <c r="E41" s="71">
+      <c r="E41" s="70">
         <v>2.5</v>
       </c>
-      <c r="F41" s="72"/>
-      <c r="G41" s="72"/>
-      <c r="H41" s="72"/>
-      <c r="I41" s="72"/>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="F41" s="71"/>
+      <c r="G41" s="71"/>
+      <c r="H41" s="71"/>
+      <c r="I41" s="71"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="51"/>
       <c r="B42" s="52"/>
       <c r="C42" s="51"/>
       <c r="D42" s="51"/>
       <c r="E42" s="51"/>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="51"/>
       <c r="B43" s="52"/>
       <c r="C43" s="51"/>
       <c r="D43" s="51"/>
       <c r="E43" s="51"/>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="51"/>
       <c r="B44" s="52"/>
       <c r="C44" s="51"/>
       <c r="D44" s="51"/>
       <c r="E44" s="51"/>
     </row>
-    <row r="45" spans="1:9" s="42" customFormat="1" ht="13.5" customHeight="1">
+    <row r="45" spans="1:9" s="42" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="35" t="s">
         <v>123</v>
       </c>
@@ -4695,7 +4688,7 @@
       <c r="D45" s="40"/>
       <c r="E45" s="40"/>
     </row>
-    <row r="46" spans="1:9" s="42" customFormat="1" ht="13.5" customHeight="1">
+    <row r="46" spans="1:9" s="42" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="40"/>
       <c r="B46" s="40"/>
       <c r="C46" s="36" t="s">
@@ -4708,7 +4701,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:9" s="42" customFormat="1" ht="13.5" customHeight="1">
+    <row r="47" spans="1:9" s="42" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="40"/>
       <c r="B47" s="2" t="s">
         <v>84</v>
@@ -4723,7 +4716,7 @@
         <v>0.27500000000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:9" s="42" customFormat="1" ht="13.5" customHeight="1">
+    <row r="48" spans="1:9" s="42" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="40"/>
       <c r="B48" s="2" t="s">
         <v>92</v>
@@ -4738,7 +4731,7 @@
         <v>0.88500000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="42" customFormat="1" ht="13.5" customHeight="1">
+    <row r="49" spans="1:5" s="42" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="40"/>
       <c r="B49" s="2" t="s">
         <v>89</v>
@@ -4753,7 +4746,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="42" customFormat="1" ht="13.5" customHeight="1">
+    <row r="50" spans="1:5" s="42" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="40"/>
       <c r="B50" s="2" t="s">
         <v>93</v>
@@ -4768,7 +4761,7 @@
         <v>0.82699999999999996</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="42" customFormat="1" ht="13.5" customHeight="1">
+    <row r="51" spans="1:5" s="42" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="40"/>
       <c r="B51" s="2" t="s">
         <v>90</v>
@@ -4783,7 +4776,7 @@
         <v>0.86899999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="42" customFormat="1" ht="13.5" customHeight="1">
+    <row r="52" spans="1:5" s="42" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="40"/>
       <c r="B52" s="2" t="s">
         <v>94</v>
@@ -4798,7 +4791,7 @@
         <v>0.68600000000000005</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="42" customFormat="1" ht="13.5" customHeight="1">
+    <row r="53" spans="1:5" s="42" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="40"/>
       <c r="B53" s="2" t="s">
         <v>91</v>
@@ -4813,7 +4806,7 @@
         <v>0.72299999999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="42" customFormat="1" ht="13.5" customHeight="1">
+    <row r="54" spans="1:5" s="42" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="40"/>
       <c r="B54" s="2" t="s">
         <v>95</v>
@@ -4828,7 +4821,7 @@
         <v>0.56299999999999994</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="42" customFormat="1" ht="13.5" customHeight="1">
+    <row r="55" spans="1:5" s="42" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="40"/>
       <c r="B55" s="2" t="s">
         <v>124</v>
@@ -4843,33 +4836,33 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="42" customFormat="1" ht="13.5" customHeight="1">
+    <row r="56" spans="1:5" s="42" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="43"/>
       <c r="B56" s="43"/>
       <c r="C56" s="43"/>
       <c r="D56" s="43"/>
       <c r="E56" s="43"/>
     </row>
-    <row r="57" spans="1:5" s="42" customFormat="1" ht="13.5" customHeight="1">
+    <row r="57" spans="1:5" s="42" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="43"/>
       <c r="B57" s="43"/>
       <c r="C57" s="43"/>
       <c r="D57" s="43"/>
       <c r="E57" s="43"/>
     </row>
-    <row r="58" spans="1:5" s="42" customFormat="1" ht="13.5" customHeight="1">
+    <row r="58" spans="1:5" s="42" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="43"/>
       <c r="B58" s="43"/>
       <c r="C58" s="43"/>
       <c r="D58" s="43"/>
       <c r="E58" s="43"/>
     </row>
-    <row r="59" spans="1:5" ht="13.5" customHeight="1">
+    <row r="59" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="13.5" customHeight="1">
+    <row r="60" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C60" s="4" t="s">
         <v>32</v>
       </c>
@@ -4880,7 +4873,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="13.5" customHeight="1">
+    <row r="61" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="2" t="s">
         <v>82</v>
       </c>
@@ -4894,7 +4887,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="13.5" customHeight="1">
+    <row r="62" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="2" t="s">
         <v>83</v>
       </c>
@@ -4908,7 +4901,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="13.5" customHeight="1">
+    <row r="63" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="2" t="s">
         <v>97</v>
       </c>
@@ -4922,7 +4915,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="15" customHeight="1">
+    <row r="64" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="2" t="s">
         <v>85</v>
       </c>
@@ -4936,7 +4929,7 @@
         <v>1.01E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B65" s="2" t="s">
         <v>86</v>
       </c>
@@ -4951,7 +4944,7 @@
       </c>
       <c r="F65" s="51"/>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B66" s="2" t="s">
         <v>87</v>
       </c>
@@ -4966,7 +4959,7 @@
       </c>
       <c r="F66" s="51"/>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B67" s="2" t="s">
         <v>120</v>
       </c>
@@ -4981,7 +4974,7 @@
       </c>
       <c r="F67" s="51"/>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B68" s="2" t="s">
         <v>121</v>
       </c>
@@ -4996,7 +4989,7 @@
       </c>
       <c r="F68" s="51"/>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B69" s="2" t="s">
         <v>98</v>
       </c>
@@ -5011,7 +5004,7 @@
       </c>
       <c r="F69" s="51"/>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="51"/>
       <c r="B70" s="52"/>
       <c r="C70" s="51"/>
@@ -5019,7 +5012,7 @@
       <c r="E70" s="51"/>
       <c r="F70" s="51"/>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="51"/>
       <c r="B71" s="52"/>
       <c r="C71" s="51"/>
@@ -5030,7 +5023,7 @@
       <c r="H71" s="51"/>
       <c r="I71" s="51"/>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="51"/>
       <c r="B72" s="52"/>
       <c r="C72" s="51"/>
@@ -5041,7 +5034,7 @@
       <c r="H72" s="51"/>
       <c r="I72" s="51"/>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>99</v>
       </c>
@@ -5050,7 +5043,7 @@
       <c r="H73" s="51"/>
       <c r="I73" s="51"/>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C74" s="4" t="s">
         <v>32</v>
       </c>
@@ -5065,7 +5058,7 @@
       <c r="H74" s="51"/>
       <c r="I74" s="51"/>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B75" s="2" t="s">
         <v>100</v>
       </c>
@@ -5083,7 +5076,7 @@
       <c r="H75" s="54"/>
       <c r="I75" s="54"/>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B76" s="2" t="s">
         <v>101</v>
       </c>
@@ -5101,7 +5094,7 @@
       <c r="H76" s="54"/>
       <c r="I76" s="54"/>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B77" s="2" t="s">
         <v>102</v>
       </c>
@@ -5116,7 +5109,7 @@
       </c>
       <c r="F77" s="51"/>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B78" s="2" t="s">
         <v>103</v>
       </c>
@@ -5134,7 +5127,7 @@
       <c r="H78" s="54"/>
       <c r="I78" s="54"/>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B79" s="2" t="s">
         <v>104</v>
       </c>
@@ -5152,7 +5145,7 @@
       <c r="H79" s="54"/>
       <c r="I79" s="54"/>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B80" s="2" t="s">
         <v>105</v>
       </c>
@@ -5170,7 +5163,7 @@
       <c r="H80" s="54"/>
       <c r="I80" s="54"/>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B81" s="2" t="s">
         <v>106</v>
       </c>
@@ -5188,7 +5181,7 @@
       <c r="H81" s="54"/>
       <c r="I81" s="54"/>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B82" s="2" t="s">
         <v>107</v>
       </c>
@@ -5206,7 +5199,7 @@
       <c r="H82" s="54"/>
       <c r="I82" s="54"/>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B83" s="2" t="s">
         <v>108</v>
       </c>
@@ -5224,7 +5217,7 @@
       <c r="H83" s="51"/>
       <c r="I83" s="51"/>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="51"/>
       <c r="B84" s="52"/>
       <c r="C84" s="51"/>
@@ -5235,7 +5228,7 @@
       <c r="H84" s="51"/>
       <c r="I84" s="51"/>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="55"/>
       <c r="B85" s="56"/>
       <c r="C85" s="57"/>
@@ -5246,7 +5239,7 @@
       <c r="H85" s="57"/>
       <c r="I85" s="51"/>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="57"/>
       <c r="B86" s="56"/>
       <c r="C86" s="58"/>
@@ -5257,7 +5250,7 @@
       <c r="H86" s="57"/>
       <c r="I86" s="51"/>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="37" t="s">
         <v>109</v>
       </c>
@@ -5269,7 +5262,7 @@
       <c r="G87" s="34"/>
       <c r="H87" s="34"/>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="34"/>
       <c r="B88" s="34"/>
       <c r="C88" s="38" t="s">
@@ -5285,7 +5278,7 @@
       <c r="G88" s="34"/>
       <c r="H88" s="34"/>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="34"/>
       <c r="B89" s="39" t="s">
         <v>110</v>
@@ -5303,7 +5296,7 @@
       <c r="G89" s="34"/>
       <c r="H89" s="34"/>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="34"/>
       <c r="B90" s="39" t="s">
         <v>111</v>
@@ -5321,7 +5314,7 @@
       <c r="G90" s="34"/>
       <c r="H90" s="34"/>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="34"/>
       <c r="B91" s="39" t="s">
         <v>112</v>
@@ -5339,7 +5332,7 @@
       <c r="G91" s="34"/>
       <c r="H91" s="34"/>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="34"/>
       <c r="B92" s="39" t="s">
         <v>113</v>
@@ -5357,7 +5350,7 @@
       <c r="G92" s="34"/>
       <c r="H92" s="34"/>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="34"/>
       <c r="B93" s="39" t="s">
         <v>114</v>
@@ -5375,7 +5368,7 @@
       <c r="G93" s="34"/>
       <c r="H93" s="34"/>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="34"/>
       <c r="B94" s="39" t="s">
         <v>115</v>
@@ -5393,7 +5386,7 @@
       <c r="G94" s="34"/>
       <c r="H94" s="34"/>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="34"/>
       <c r="B95" s="39" t="s">
         <v>116</v>
@@ -5411,30 +5404,25 @@
       <c r="G95" s="34"/>
       <c r="H95" s="34"/>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F96" s="34"/>
       <c r="G96" s="34"/>
       <c r="H96" s="34"/>
     </row>
-    <row r="97" spans="6:8">
+    <row r="97" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F97" s="34"/>
       <c r="G97" s="34"/>
       <c r="H97" s="34"/>
     </row>
-    <row r="98" spans="6:8" ht="13.5" customHeight="1">
+    <row r="98" spans="6:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F98" s="34"/>
       <c r="G98" s="34"/>
       <c r="H98" s="34"/>
     </row>
-    <row r="99" spans="6:8" ht="13.5" customHeight="1"/>
+    <row r="99" spans="6:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5446,14 +5434,14 @@
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
@@ -5473,7 +5461,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B3" s="4">
         <v>1</v>
       </c>
@@ -5496,7 +5484,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" s="4">
         <v>2</v>
       </c>
@@ -5519,7 +5507,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" s="4">
         <v>3</v>
       </c>
@@ -5542,7 +5530,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" s="4">
         <v>6</v>
       </c>
@@ -5565,7 +5553,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" s="4">
         <v>7</v>
       </c>
@@ -5588,7 +5576,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="4">
         <v>6</v>
       </c>
@@ -5611,7 +5599,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" s="4">
         <v>7</v>
       </c>
@@ -5634,7 +5622,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" s="4">
         <v>8</v>
       </c>
@@ -5657,7 +5645,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" s="4">
         <v>9</v>
       </c>
@@ -5683,11 +5671,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5699,15 +5682,15 @@
       <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D2" s="4">
         <v>2000</v>
       </c>
@@ -5775,7 +5758,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5809,7 +5792,7 @@
       </c>
       <c r="Z3" s="7"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5865,7 +5848,7 @@
       </c>
       <c r="Z4" s="7"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5899,7 +5882,7 @@
       </c>
       <c r="Z5" s="7"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5933,7 +5916,7 @@
       </c>
       <c r="Z7" s="7"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5989,7 +5972,7 @@
       </c>
       <c r="Z8" s="7"/>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6023,7 +6006,7 @@
       </c>
       <c r="Z9" s="7"/>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6057,7 +6040,7 @@
       </c>
       <c r="Z11" s="7"/>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6113,7 +6096,7 @@
       </c>
       <c r="Z12" s="7"/>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6147,7 +6130,7 @@
       </c>
       <c r="Z13" s="7"/>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -6160,7 +6143,7 @@
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -6194,7 +6177,7 @@
       </c>
       <c r="Z15" s="7"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -6250,7 +6233,7 @@
       </c>
       <c r="Z16" s="7"/>
     </row>
-    <row r="17" spans="2:26">
+    <row r="17" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -6284,7 +6267,7 @@
       </c>
       <c r="Z17" s="7"/>
     </row>
-    <row r="19" spans="2:26">
+    <row r="19" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -6318,7 +6301,7 @@
       </c>
       <c r="Z19" s="7"/>
     </row>
-    <row r="20" spans="2:26">
+    <row r="20" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -6374,7 +6357,7 @@
       </c>
       <c r="Z20" s="7"/>
     </row>
-    <row r="21" spans="2:26">
+    <row r="21" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B21" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -6408,7 +6391,7 @@
       </c>
       <c r="Z21" s="7"/>
     </row>
-    <row r="23" spans="2:26">
+    <row r="23" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -6442,7 +6425,7 @@
       </c>
       <c r="Z23" s="7"/>
     </row>
-    <row r="24" spans="2:26">
+    <row r="24" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B24" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -6498,7 +6481,7 @@
       </c>
       <c r="Z24" s="7"/>
     </row>
-    <row r="25" spans="2:26">
+    <row r="25" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B25" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -6532,7 +6515,7 @@
       </c>
       <c r="Z25" s="7"/>
     </row>
-    <row r="27" spans="2:26">
+    <row r="27" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B27" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -6566,7 +6549,7 @@
       </c>
       <c r="Z27" s="7"/>
     </row>
-    <row r="28" spans="2:26">
+    <row r="28" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B28" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -6622,7 +6605,7 @@
       </c>
       <c r="Z28" s="7"/>
     </row>
-    <row r="29" spans="2:26">
+    <row r="29" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B29" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -6656,7 +6639,7 @@
       </c>
       <c r="Z29" s="7"/>
     </row>
-    <row r="31" spans="2:26">
+    <row r="31" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B31" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -6690,7 +6673,7 @@
       </c>
       <c r="Z31" s="7"/>
     </row>
-    <row r="32" spans="2:26">
+    <row r="32" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B32" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -6756,7 +6739,7 @@
       </c>
       <c r="Z32" s="7"/>
     </row>
-    <row r="33" spans="2:26">
+    <row r="33" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B33" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -6790,7 +6773,7 @@
       </c>
       <c r="Z33" s="7"/>
     </row>
-    <row r="35" spans="2:26">
+    <row r="35" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B35" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -6824,7 +6807,7 @@
       </c>
       <c r="Z35" s="7"/>
     </row>
-    <row r="36" spans="2:26">
+    <row r="36" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B36" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -6890,7 +6873,7 @@
       </c>
       <c r="Z36" s="7"/>
     </row>
-    <row r="37" spans="2:26">
+    <row r="37" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B37" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -6927,11 +6910,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -6943,14 +6921,14 @@
       <selection activeCell="Z37" sqref="Z37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D2" s="4">
         <v>2000</v>
       </c>
@@ -7018,7 +6996,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -7058,7 +7036,7 @@
       </c>
       <c r="Z3" s="12"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -7098,7 +7076,7 @@
       </c>
       <c r="Z4" s="12"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -7138,7 +7116,7 @@
       </c>
       <c r="Z5" s="12"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -7172,7 +7150,7 @@
       </c>
       <c r="Z7" s="12"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -7208,7 +7186,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -7242,7 +7220,7 @@
       </c>
       <c r="Z9" s="12"/>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7278,7 +7256,7 @@
       </c>
       <c r="Z11" s="12"/>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7320,7 +7298,7 @@
       </c>
       <c r="Z12" s="12"/>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7356,7 +7334,7 @@
       </c>
       <c r="Z13" s="12"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -7390,7 +7368,7 @@
       </c>
       <c r="Z15" s="12"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -7426,7 +7404,7 @@
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="17" spans="2:26">
+    <row r="17" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -7460,7 +7438,7 @@
       </c>
       <c r="Z17" s="12"/>
     </row>
-    <row r="19" spans="2:26">
+    <row r="19" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -7494,7 +7472,7 @@
       </c>
       <c r="Z19" s="12"/>
     </row>
-    <row r="20" spans="2:26">
+    <row r="20" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -7530,7 +7508,7 @@
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="21" spans="2:26">
+    <row r="21" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B21" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -7564,7 +7542,7 @@
       </c>
       <c r="Z21" s="12"/>
     </row>
-    <row r="23" spans="2:26">
+    <row r="23" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -7598,7 +7576,7 @@
       </c>
       <c r="Z23" s="12"/>
     </row>
-    <row r="24" spans="2:26">
+    <row r="24" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B24" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -7646,7 +7624,7 @@
       </c>
       <c r="Z24" s="12"/>
     </row>
-    <row r="25" spans="2:26">
+    <row r="25" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B25" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -7680,7 +7658,7 @@
       </c>
       <c r="Z25" s="12"/>
     </row>
-    <row r="27" spans="2:26">
+    <row r="27" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B27" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -7714,7 +7692,7 @@
       </c>
       <c r="Z27" s="12"/>
     </row>
-    <row r="28" spans="2:26">
+    <row r="28" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B28" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -7762,7 +7740,7 @@
       </c>
       <c r="Z28" s="12"/>
     </row>
-    <row r="29" spans="2:26">
+    <row r="29" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B29" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -7796,7 +7774,7 @@
       </c>
       <c r="Z29" s="12"/>
     </row>
-    <row r="31" spans="2:26">
+    <row r="31" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B31" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -7830,7 +7808,7 @@
       </c>
       <c r="Z31" s="12"/>
     </row>
-    <row r="32" spans="2:26">
+    <row r="32" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B32" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -7869,7 +7847,7 @@
         <v>8.4000000000000003E-4</v>
       </c>
     </row>
-    <row r="33" spans="2:26">
+    <row r="33" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B33" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -7903,7 +7881,7 @@
       </c>
       <c r="Z33" s="12"/>
     </row>
-    <row r="35" spans="2:26">
+    <row r="35" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B35" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -7937,7 +7915,7 @@
       </c>
       <c r="Z35" s="12"/>
     </row>
-    <row r="36" spans="2:26">
+    <row r="36" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B36" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -7976,7 +7954,7 @@
         <v>1.2899999999999999E-3</v>
       </c>
     </row>
-    <row r="37" spans="2:26">
+    <row r="37" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B37" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -8013,11 +7991,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8029,14 +8002,14 @@
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C2" s="4">
         <v>2000</v>
       </c>
@@ -8104,7 +8077,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -8137,7 +8110,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -8170,7 +8143,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -8203,7 +8176,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -8236,7 +8209,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -8269,7 +8242,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -8302,7 +8275,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -8335,7 +8308,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -8368,7 +8341,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -8401,12 +8374,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C16" s="4">
         <v>2000</v>
       </c>
@@ -8474,7 +8447,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -8507,7 +8480,7 @@
       </c>
       <c r="Y17" s="12"/>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -8540,7 +8513,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -8573,7 +8546,7 @@
       </c>
       <c r="Y19" s="12"/>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -8606,7 +8579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B21" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -8639,7 +8612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B22" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -8672,7 +8645,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -8705,7 +8678,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B24" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -8738,7 +8711,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B25" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -8771,12 +8744,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C30" s="4">
         <v>2000</v>
       </c>
@@ -8844,7 +8817,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B31" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -8877,7 +8850,7 @@
       </c>
       <c r="Y31" s="12"/>
     </row>
-    <row r="32" spans="1:25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B32" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -8910,7 +8883,7 @@
       </c>
       <c r="Y32" s="12"/>
     </row>
-    <row r="33" spans="2:25">
+    <row r="33" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B33" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -8943,7 +8916,7 @@
       </c>
       <c r="Y33" s="12"/>
     </row>
-    <row r="34" spans="2:25">
+    <row r="34" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B34" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -8976,7 +8949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:25">
+    <row r="35" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B35" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -9009,7 +8982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:25">
+    <row r="36" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B36" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -9042,7 +9015,7 @@
       </c>
       <c r="Y36" s="12"/>
     </row>
-    <row r="37" spans="2:25">
+    <row r="37" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B37" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -9075,7 +9048,7 @@
       </c>
       <c r="Y37" s="12"/>
     </row>
-    <row r="38" spans="2:25">
+    <row r="38" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B38" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -9108,7 +9081,7 @@
       </c>
       <c r="Y38" s="12"/>
     </row>
-    <row r="39" spans="2:25">
+    <row r="39" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B39" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -9144,11 +9117,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -9156,18 +9124,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y64"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C2" s="4">
         <v>2000</v>
       </c>
@@ -9235,7 +9203,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -9270,7 +9238,7 @@
       </c>
       <c r="Y3" s="15"/>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -9307,7 +9275,7 @@
       </c>
       <c r="Y4" s="15"/>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -9340,7 +9308,7 @@
       </c>
       <c r="Y5" s="15"/>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -9373,7 +9341,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -9406,7 +9374,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -9443,7 +9411,7 @@
       </c>
       <c r="Y8" s="15"/>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -9480,7 +9448,7 @@
       </c>
       <c r="Y9" s="15"/>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -9513,7 +9481,7 @@
       </c>
       <c r="Y10" s="15"/>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -9546,12 +9514,12 @@
       </c>
       <c r="Y11" s="15"/>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C16" s="4">
         <v>2000</v>
       </c>
@@ -9619,7 +9587,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
         <v>40</v>
       </c>
@@ -9651,12 +9619,12 @@
       </c>
       <c r="Y17" s="5"/>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C22" s="4">
         <v>2000</v>
       </c>
@@ -9724,7 +9692,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="s">
         <v>42</v>
       </c>
@@ -9772,12 +9740,12 @@
       </c>
       <c r="Y23" s="5"/>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" s="67" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C28" s="4">
         <v>2000</v>
       </c>
@@ -9845,7 +9813,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B29" s="4" t="s">
         <v>42</v>
       </c>
@@ -9881,12 +9849,12 @@
       </c>
       <c r="Y29" s="5"/>
     </row>
-    <row r="33" spans="1:25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C34" s="4">
         <v>2000</v>
       </c>
@@ -9954,7 +9922,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B35" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -9987,7 +9955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B36" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -10020,7 +9988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B37" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -10053,7 +10021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B38" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -10086,7 +10054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B39" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -10119,7 +10087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B40" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -10152,7 +10120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B41" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -10185,7 +10153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B42" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -10218,7 +10186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B43" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -10251,12 +10219,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C48" s="4">
         <v>2000</v>
       </c>
@@ -10324,7 +10292,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B49" s="4" t="s">
         <v>42</v>
       </c>
@@ -10358,12 +10326,12 @@
       </c>
       <c r="Y49" s="5"/>
     </row>
-    <row r="53" spans="1:25">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C54" s="4">
         <v>2000</v>
       </c>
@@ -10431,7 +10399,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B55" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -10484,7 +10452,7 @@
       </c>
       <c r="Y55" s="20"/>
     </row>
-    <row r="56" spans="1:25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B56" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -10517,7 +10485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B57" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -10570,7 +10538,7 @@
       </c>
       <c r="Y57" s="20"/>
     </row>
-    <row r="58" spans="1:25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B58" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -10603,12 +10571,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:25">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="1:25">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C63" s="4">
         <v>2000</v>
       </c>
@@ -10676,7 +10644,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="64" spans="1:25">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B64" s="4" t="s">
         <v>42</v>
       </c>
@@ -10711,11 +10679,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -10727,14 +10690,14 @@
       <selection activeCell="A40" sqref="A40:XFD70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C2" s="4">
         <v>2000</v>
       </c>
@@ -10802,7 +10765,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>42</v>
       </c>
@@ -10846,12 +10809,12 @@
       </c>
       <c r="Y3" s="20"/>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C8" s="4">
         <v>2000</v>
       </c>
@@ -10919,7 +10882,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>42</v>
       </c>
@@ -10953,12 +10916,12 @@
       </c>
       <c r="Y9" s="20"/>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C14" s="4">
         <v>2000</v>
       </c>
@@ -11026,7 +10989,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
         <v>42</v>
       </c>
@@ -11084,12 +11047,12 @@
       </c>
       <c r="Y15" s="20"/>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C20" s="4">
         <v>2000</v>
       </c>
@@ -11157,7 +11120,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B21" s="4" t="s">
         <v>42</v>
       </c>
@@ -11215,7 +11178,7 @@
       </c>
       <c r="Y21" s="28"/>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
         <v>51</v>
       </c>
@@ -11244,7 +11207,7 @@
       <c r="X25" s="22"/>
       <c r="Y25" s="22"/>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" s="22"/>
       <c r="B26" s="22"/>
       <c r="C26" s="23">
@@ -11315,7 +11278,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" s="22"/>
       <c r="B27" s="23" t="s">
         <v>42</v>
@@ -11346,12 +11309,12 @@
       </c>
       <c r="Y27" s="29"/>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C32" s="4">
         <v>2000</v>
       </c>
@@ -11419,7 +11382,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B33" s="4" t="s">
         <v>42</v>
       </c>
@@ -11477,12 +11440,12 @@
       </c>
       <c r="Y33" s="20"/>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C38" s="4">
         <v>2000</v>
       </c>
@@ -11550,7 +11513,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B39" s="4" t="s">
         <v>42</v>
       </c>
@@ -11588,12 +11551,12 @@
       </c>
       <c r="Y39" s="20"/>
     </row>
-    <row r="43" spans="1:25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A43" s="59" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C44" s="60">
         <v>2000</v>
       </c>
@@ -11661,7 +11624,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B45" s="60" t="s">
         <v>40</v>
       </c>
@@ -11691,12 +11654,12 @@
       </c>
       <c r="Y45" s="61"/>
     </row>
-    <row r="49" spans="1:25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A49" s="59" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="50" spans="1:25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C50" s="60">
         <v>2000</v>
       </c>
@@ -11764,7 +11727,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="1:25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B51" s="60" t="s">
         <v>40</v>
       </c>
@@ -11794,12 +11757,12 @@
       </c>
       <c r="Y51" s="61"/>
     </row>
-    <row r="55" spans="1:25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A55" s="59" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="56" spans="1:25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C56" s="60">
         <v>2000</v>
       </c>
@@ -11867,7 +11830,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B57" s="60" t="s">
         <v>40</v>
       </c>
@@ -11897,12 +11860,12 @@
       </c>
       <c r="Y57" s="61"/>
     </row>
-    <row r="61" spans="1:25">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A61" s="59" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="62" spans="1:25">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C62" s="60">
         <v>2000</v>
       </c>
@@ -11970,7 +11933,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="63" spans="1:25">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B63" s="60" t="s">
         <v>40</v>
       </c>
@@ -12000,12 +11963,12 @@
       </c>
       <c r="Y63" s="61"/>
     </row>
-    <row r="67" spans="1:25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A67" s="59" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="68" spans="1:25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C68" s="60">
         <v>2000</v>
       </c>
@@ -12073,7 +12036,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="69" spans="1:25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B69" s="60" t="s">
         <v>40</v>
       </c>
@@ -12106,11 +12069,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -12118,18 +12076,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="22"/>
       <c r="C2" s="4">
         <v>2000</v>
@@ -12198,7 +12156,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="22"/>
       <c r="B3" s="4" t="str">
         <f>Populations!$C$3</f>
@@ -12232,7 +12190,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="22"/>
       <c r="B4" s="4" t="str">
         <f>Populations!$C$4</f>
@@ -12266,7 +12224,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -12299,7 +12257,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -12332,7 +12290,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -12365,7 +12323,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -12398,7 +12356,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="22"/>
       <c r="B9" s="4" t="str">
         <f>Populations!$C$9</f>
@@ -12432,7 +12390,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="22"/>
       <c r="B10" s="4" t="str">
         <f>Populations!$C$10</f>
@@ -12466,7 +12424,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="22"/>
       <c r="B11" s="4" t="str">
         <f>Populations!$C$11</f>
@@ -12500,12 +12458,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="64" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C16" s="4">
         <v>2000</v>
       </c>
@@ -12573,7 +12531,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
         <v>40</v>
       </c>
@@ -12605,7 +12563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -12641,7 +12599,7 @@
       <c r="AH18" s="4"/>
       <c r="AI18" s="4"/>
     </row>
-    <row r="19" spans="1:35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -12677,7 +12635,7 @@
       <c r="AH19" s="4"/>
       <c r="AI19" s="4"/>
     </row>
-    <row r="20" spans="1:35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -12713,12 +12671,12 @@
       <c r="AH20" s="4"/>
       <c r="AI20" s="4"/>
     </row>
-    <row r="21" spans="1:35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
       <c r="C22" s="4">
         <v>2000</v>
       </c>
@@ -12786,7 +12744,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -12819,7 +12777,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="24" spans="1:35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B24" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -12852,7 +12810,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="25" spans="1:35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B25" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -12885,7 +12843,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="26" spans="1:35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B26" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -12918,7 +12876,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="27" spans="1:35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B27" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -12951,7 +12909,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="28" spans="1:35">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B28" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -12984,7 +12942,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="29" spans="1:35">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B29" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -13017,7 +12975,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="30" spans="1:35">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B30" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -13050,7 +13008,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="31" spans="1:35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B31" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -13083,12 +13041,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="35" spans="1:35">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="1:35">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.2">
       <c r="C36" s="4">
         <v>2000</v>
       </c>
@@ -13156,7 +13114,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:35">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B37" s="4" t="s">
         <v>40</v>
       </c>
@@ -13188,7 +13146,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="38" spans="1:35">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -13224,7 +13182,7 @@
       <c r="AH38" s="4"/>
       <c r="AI38" s="4"/>
     </row>
-    <row r="39" spans="1:35">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
@@ -13260,7 +13218,7 @@
       <c r="AH39" s="4"/>
       <c r="AI39" s="4"/>
     </row>
-    <row r="40" spans="1:35">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
@@ -13296,7 +13254,7 @@
       <c r="AH40" s="4"/>
       <c r="AI40" s="4"/>
     </row>
-    <row r="41" spans="1:35">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
         <v>55</v>
       </c>
@@ -13325,7 +13283,7 @@
       <c r="X41" s="22"/>
       <c r="Y41" s="22"/>
     </row>
-    <row r="42" spans="1:35">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A42" s="22"/>
       <c r="B42" s="22"/>
       <c r="C42" s="23">
@@ -13396,25 +13354,52 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:35">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A43" s="22"/>
       <c r="B43" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="31"/>
+      <c r="C43" s="31">
+        <f>'Testing &amp; treatment'!C23</f>
+        <v>0</v>
+      </c>
       <c r="D43" s="31"/>
       <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
+      <c r="F43" s="31">
+        <f>'Testing &amp; treatment'!F23</f>
+        <v>1</v>
+      </c>
       <c r="G43" s="31"/>
       <c r="H43" s="31"/>
       <c r="I43" s="31"/>
-      <c r="J43" s="31"/>
-      <c r="K43" s="31"/>
-      <c r="L43" s="31"/>
-      <c r="M43" s="31"/>
-      <c r="N43" s="31"/>
-      <c r="O43" s="31"/>
-      <c r="P43" s="31"/>
+      <c r="J43" s="31">
+        <f>'Testing &amp; treatment'!J23</f>
+        <v>616</v>
+      </c>
+      <c r="K43" s="31">
+        <f>'Testing &amp; treatment'!K23</f>
+        <v>1160</v>
+      </c>
+      <c r="L43" s="31">
+        <f>'Testing &amp; treatment'!L23</f>
+        <v>1996</v>
+      </c>
+      <c r="M43" s="31">
+        <f>'Testing &amp; treatment'!M23</f>
+        <v>2122</v>
+      </c>
+      <c r="N43" s="31">
+        <f>'Testing &amp; treatment'!N23</f>
+        <v>2377</v>
+      </c>
+      <c r="O43" s="31">
+        <f>'Testing &amp; treatment'!O23</f>
+        <v>2575</v>
+      </c>
+      <c r="P43" s="31">
+        <f>'Testing &amp; treatment'!P23</f>
+        <v>3308</v>
+      </c>
       <c r="Q43" s="31"/>
       <c r="R43" s="31"/>
       <c r="S43" s="31"/>
@@ -13425,18 +13410,11 @@
       <c r="X43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="Y43" s="32">
-        <v>1</v>
-      </c>
+      <c r="Y43" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -13448,14 +13426,14 @@
       <selection activeCell="A95" sqref="A95:XFD102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C2" s="4">
         <v>2000</v>
       </c>
@@ -13523,7 +13501,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -13556,7 +13534,7 @@
       </c>
       <c r="Y3" s="5"/>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -13589,7 +13567,7 @@
       </c>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -13622,7 +13600,7 @@
       </c>
       <c r="Y5" s="5"/>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -13655,7 +13633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -13688,7 +13666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -13721,7 +13699,7 @@
       </c>
       <c r="Y8" s="5"/>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -13754,7 +13732,7 @@
       </c>
       <c r="Y9" s="5"/>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -13787,7 +13765,7 @@
       </c>
       <c r="Y10" s="5"/>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -13820,12 +13798,12 @@
       </c>
       <c r="Y11" s="5"/>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C16" s="4">
         <v>2000</v>
       </c>
@@ -13893,7 +13871,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -13926,7 +13904,7 @@
       </c>
       <c r="Y17" s="5"/>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -13959,7 +13937,7 @@
       </c>
       <c r="Y18" s="5"/>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -13992,7 +13970,7 @@
       </c>
       <c r="Y19" s="5"/>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -14025,7 +14003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B21" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -14058,7 +14036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B22" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -14091,7 +14069,7 @@
       </c>
       <c r="Y22" s="5"/>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -14124,7 +14102,7 @@
       </c>
       <c r="Y23" s="5"/>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B24" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -14157,7 +14135,7 @@
       </c>
       <c r="Y24" s="5"/>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B25" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -14190,12 +14168,12 @@
       </c>
       <c r="Y25" s="5"/>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C30" s="4">
         <v>2000</v>
       </c>
@@ -14263,7 +14241,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B31" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -14296,7 +14274,7 @@
       </c>
       <c r="Y31" s="5"/>
     </row>
-    <row r="32" spans="1:25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B32" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -14329,7 +14307,7 @@
       </c>
       <c r="Y32" s="5"/>
     </row>
-    <row r="33" spans="1:25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B33" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -14362,7 +14340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B34" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -14395,7 +14373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B35" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -14428,7 +14406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B36" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -14461,7 +14439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B37" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -14494,7 +14472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B38" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -14527,7 +14505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B39" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -14560,12 +14538,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="1:25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C44" s="4">
         <v>2000</v>
       </c>
@@ -14633,7 +14611,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -14666,7 +14644,7 @@
       </c>
       <c r="Y45" s="15"/>
     </row>
-    <row r="46" spans="1:25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B46" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -14699,7 +14677,7 @@
       </c>
       <c r="Y46" s="15"/>
     </row>
-    <row r="47" spans="1:25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B47" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -14732,7 +14710,7 @@
       </c>
       <c r="Y47" s="15"/>
     </row>
-    <row r="48" spans="1:25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B48" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -14765,7 +14743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B49" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -14798,7 +14776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B50" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -14831,7 +14809,7 @@
       </c>
       <c r="Y50" s="15"/>
     </row>
-    <row r="51" spans="1:25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B51" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -14864,7 +14842,7 @@
       </c>
       <c r="Y51" s="15"/>
     </row>
-    <row r="52" spans="1:25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B52" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -14897,7 +14875,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:25">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B53" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -14930,12 +14908,12 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C58" s="4">
         <v>2000</v>
       </c>
@@ -15003,7 +14981,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="1:25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B59" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -15036,7 +15014,7 @@
       </c>
       <c r="Y59" s="15"/>
     </row>
-    <row r="60" spans="1:25">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B60" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -15073,7 +15051,7 @@
       </c>
       <c r="Y60" s="15"/>
     </row>
-    <row r="61" spans="1:25">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B61" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -15106,7 +15084,7 @@
       </c>
       <c r="Y61" s="15"/>
     </row>
-    <row r="62" spans="1:25">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B62" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -15139,7 +15117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:25">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B63" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -15172,7 +15150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:25">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B64" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -15209,7 +15187,7 @@
       </c>
       <c r="Y64" s="15"/>
     </row>
-    <row r="65" spans="1:25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B65" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -15246,7 +15224,7 @@
       </c>
       <c r="Y65" s="15"/>
     </row>
-    <row r="66" spans="1:25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B66" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -15279,7 +15257,7 @@
       </c>
       <c r="Y66" s="15"/>
     </row>
-    <row r="67" spans="1:25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B67" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -15312,12 +15290,12 @@
       </c>
       <c r="Y67" s="15"/>
     </row>
-    <row r="71" spans="1:25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="72" spans="1:25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C72" s="4">
         <v>2000</v>
       </c>
@@ -15385,7 +15363,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="73" spans="1:25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B73" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -15420,7 +15398,7 @@
       </c>
       <c r="Y73" s="15"/>
     </row>
-    <row r="74" spans="1:25">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B74" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -15453,7 +15431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B75" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -15486,7 +15464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B76" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -15519,7 +15497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B77" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -15552,7 +15530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:25">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B78" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -15585,7 +15563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B79" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>F 15-49</v>
@@ -15618,7 +15596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:25">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B80" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -15651,7 +15629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:25">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B81" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>F 50+</v>
@@ -15684,12 +15662,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:25">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="86" spans="1:25">
+    <row r="86" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C86" s="4">
         <v>2000</v>
       </c>
@@ -15757,7 +15735,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="1:25">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B87" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -15790,7 +15768,7 @@
       </c>
       <c r="Y87" s="15"/>
     </row>
-    <row r="88" spans="1:25">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B88" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -15823,7 +15801,7 @@
       </c>
       <c r="Y88" s="15"/>
     </row>
-    <row r="89" spans="1:25">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B89" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -15856,7 +15834,7 @@
       </c>
       <c r="Y89" s="15"/>
     </row>
-    <row r="90" spans="1:25">
+    <row r="90" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B90" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>M 15-49</v>
@@ -15889,7 +15867,7 @@
       </c>
       <c r="Y90" s="15"/>
     </row>
-    <row r="91" spans="1:25">
+    <row r="91" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B91" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>M 50+</v>
@@ -15927,10 +15905,5 @@
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
going to do it the same way as concentrated
</commit_message>
<xml_diff>
--- a/tests/generalized.xlsx
+++ b/tests/generalized.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="16640" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="16640" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -13207,8 +13207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S27" sqref="S27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16425,8 +16425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fixed upper age limit
</commit_message>
<xml_diff>
--- a/tests/generalized.xlsx
+++ b/tests/generalized.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/optima/tests/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="16640" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="28560" windowHeight="16320" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -25,11 +20,8 @@
     <sheet name="Partnerships &amp; transitions" sheetId="11" r:id="rId11"/>
     <sheet name="Constants" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -640,7 +632,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -675,7 +667,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -890,26 +882,26 @@
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="80.59765625" customWidth="1"/>
+    <col min="1" max="1" width="80.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:1" ht="65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -955,7 +947,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -2077,9 +2069,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="15" width="12.59765625" customWidth="1"/>
+    <col min="3" max="15" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
@@ -3609,7 +3601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>Females 0-9</v>
@@ -3654,7 +3646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>Males 10-19</v>
@@ -3699,7 +3691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>Females 10-19</v>
@@ -3744,7 +3736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>Males 20-24</v>
@@ -3789,7 +3781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>Females 20-24</v>
@@ -3834,7 +3826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="str">
         <f>Populations!$C$12</f>
         <v>Males 25-49</v>
@@ -3879,7 +3871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="str">
         <f>Populations!$C$13</f>
         <v>Females 25-49</v>
@@ -3924,7 +3916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="str">
         <f>Populations!$C$14</f>
         <v>Males 50+</v>
@@ -3969,7 +3961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="str">
         <f>Populations!$C$15</f>
         <v>Females 50+</v>
@@ -4014,12 +4006,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C56" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -4073,7 +4065,7 @@
         <v>Females 50+</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B57" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -4118,7 +4110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B58" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -4163,7 +4155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B59" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -4208,7 +4200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B60" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>Males 0-9</v>
@@ -4253,7 +4245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B61" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>Females 0-9</v>
@@ -4298,7 +4290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>Males 10-19</v>
@@ -4343,7 +4335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>Females 10-19</v>
@@ -4388,7 +4380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>Males 20-24</v>
@@ -4433,7 +4425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>Females 20-24</v>
@@ -4478,7 +4470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B66" s="4" t="str">
         <f>Populations!$C$12</f>
         <v>Males 25-49</v>
@@ -4523,7 +4515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B67" s="4" t="str">
         <f>Populations!$C$13</f>
         <v>Females 25-49</v>
@@ -4568,7 +4560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B68" s="4" t="str">
         <f>Populations!$C$14</f>
         <v>Males 50+</v>
@@ -4613,7 +4605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B69" s="4" t="str">
         <f>Populations!$C$15</f>
         <v>Females 50+</v>
@@ -4658,12 +4650,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C74" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -4717,7 +4709,7 @@
         <v>Females 50+</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -4762,7 +4754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B76" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>Females 0-9</v>
@@ -4807,7 +4799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B77" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>Females 10-19</v>
@@ -4852,7 +4844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B78" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>Females 20-24</v>
@@ -4897,7 +4889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B79" s="4" t="str">
         <f>Populations!$C$13</f>
         <v>Females 25-49</v>
@@ -4942,7 +4934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B80" s="4" t="str">
         <f>Populations!$C$15</f>
         <v>Females 50+</v>
@@ -4987,12 +4979,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C85" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5046,7 +5038,7 @@
         <v>Females 50+</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B86" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5091,7 +5083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B87" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5136,7 +5128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B88" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5181,7 +5173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B89" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>Males 0-9</v>
@@ -5226,7 +5218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B90" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>Females 0-9</v>
@@ -5271,7 +5263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B91" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>Males 10-19</v>
@@ -5316,7 +5308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B92" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>Females 10-19</v>
@@ -5361,7 +5353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B93" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>Males 20-24</v>
@@ -5406,7 +5398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B94" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>Females 20-24</v>
@@ -5451,7 +5443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B95" s="4" t="str">
         <f>Populations!$C$12</f>
         <v>Males 25-49</v>
@@ -5496,7 +5488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B96" s="4" t="str">
         <f>Populations!$C$13</f>
         <v>Females 25-49</v>
@@ -5541,7 +5533,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B97" s="4" t="str">
         <f>Populations!$C$14</f>
         <v>Males 50+</v>
@@ -5586,7 +5578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B98" s="4" t="str">
         <f>Populations!$C$15</f>
         <v>Females 50+</v>
@@ -5631,12 +5623,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C103" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5690,7 +5682,7 @@
         <v>Females 50+</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B104" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5735,7 +5727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B105" s="4" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5780,7 +5772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B106" s="4" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5825,7 +5817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B107" s="4" t="str">
         <f>Populations!$C$6</f>
         <v>Males 0-9</v>
@@ -5870,7 +5862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B108" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>Females 0-9</v>
@@ -5915,7 +5907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B109" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>Males 10-19</v>
@@ -5960,7 +5952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B110" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>Females 10-19</v>
@@ -6005,7 +5997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B111" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>Males 20-24</v>
@@ -6050,7 +6042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B112" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>Females 20-24</v>
@@ -6095,7 +6087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B113" s="4" t="str">
         <f>Populations!$C$12</f>
         <v>Males 25-49</v>
@@ -6140,7 +6132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B114" s="4" t="str">
         <f>Populations!$C$13</f>
         <v>Females 25-49</v>
@@ -6185,7 +6177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B115" s="4" t="str">
         <f>Populations!$C$14</f>
         <v>Males 50+</v>
@@ -6230,7 +6222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B116" s="4" t="str">
         <f>Populations!$C$15</f>
         <v>Females 50+</v>
@@ -6286,9 +6278,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="40.59765625" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -6691,12 +6683,12 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C46" s="4" t="s">
         <v>42</v>
       </c>
@@ -6707,7 +6699,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
         <v>103</v>
       </c>
@@ -6721,7 +6713,7 @@
         <v>0.27500000000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
         <v>113</v>
       </c>
@@ -6735,7 +6727,7 @@
         <v>0.88500000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
         <v>109</v>
       </c>
@@ -6749,7 +6741,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
         <v>114</v>
       </c>
@@ -6763,7 +6755,7 @@
         <v>0.82699999999999996</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
         <v>110</v>
       </c>
@@ -6777,7 +6769,7 @@
         <v>0.86899999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
         <v>115</v>
       </c>
@@ -6791,7 +6783,7 @@
         <v>0.68600000000000005</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
         <v>111</v>
       </c>
@@ -6805,7 +6797,7 @@
         <v>0.72299999999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
         <v>116</v>
       </c>
@@ -6819,7 +6811,7 @@
         <v>0.56299999999999994</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
         <v>120</v>
       </c>
@@ -6833,12 +6825,12 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C60" s="4" t="s">
         <v>42</v>
       </c>
@@ -6849,7 +6841,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
         <v>101</v>
       </c>
@@ -6863,7 +6855,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
         <v>102</v>
       </c>
@@ -6877,7 +6869,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
         <v>122</v>
       </c>
@@ -6891,7 +6883,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
         <v>104</v>
       </c>
@@ -6905,7 +6897,7 @@
         <v>1.01E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
         <v>105</v>
       </c>
@@ -6919,7 +6911,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
         <v>106</v>
       </c>
@@ -6933,7 +6925,7 @@
         <v>0.432</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="s">
         <v>123</v>
       </c>
@@ -6947,7 +6939,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
         <v>124</v>
       </c>
@@ -6961,7 +6953,7 @@
         <v>0.8417</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
         <v>125</v>
       </c>
@@ -6975,12 +6967,12 @@
         <v>3.71</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C74" s="4" t="s">
         <v>42</v>
       </c>
@@ -6991,7 +6983,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="s">
         <v>127</v>
       </c>
@@ -7005,7 +6997,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
         <v>128</v>
       </c>
@@ -7019,7 +7011,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B77" s="3" t="s">
         <v>129</v>
       </c>
@@ -7033,7 +7025,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
         <v>130</v>
       </c>
@@ -7047,7 +7039,7 @@
         <v>5.19</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
         <v>131</v>
       </c>
@@ -7061,7 +7053,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B80" s="3" t="s">
         <v>132</v>
       </c>
@@ -7075,7 +7067,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="s">
         <v>133</v>
       </c>
@@ -7089,7 +7081,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="s">
         <v>134</v>
       </c>
@@ -7103,7 +7095,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B83" s="3" t="s">
         <v>135</v>
       </c>
@@ -7117,12 +7109,12 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C88" s="4" t="s">
         <v>42</v>
       </c>
@@ -7133,7 +7125,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B89" s="3" t="s">
         <v>137</v>
       </c>
@@ -7147,7 +7139,7 @@
         <v>0.20499999999999999</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B90" s="3" t="s">
         <v>138</v>
       </c>
@@ -7161,7 +7153,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="s">
         <v>139</v>
       </c>
@@ -7175,7 +7167,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B92" s="3" t="s">
         <v>140</v>
       </c>
@@ -7189,7 +7181,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B93" s="3" t="s">
         <v>141</v>
       </c>
@@ -7203,7 +7195,7 @@
         <v>0.47399999999999998</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="s">
         <v>142</v>
       </c>
@@ -7217,7 +7209,7 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B95" s="3" t="s">
         <v>143</v>
       </c>
@@ -7240,15 +7232,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.59765625" customWidth="1"/>
-    <col min="4" max="4" width="40.59765625" customWidth="1"/>
-    <col min="7" max="7" width="12.59765625" customWidth="1"/>
-    <col min="8" max="9" width="16.59765625" customWidth="1"/>
-    <col min="10" max="10" width="12.59765625" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="40.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="8" max="9" width="16.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -7549,7 +7543,7 @@
         <v>50</v>
       </c>
       <c r="H14" s="5">
-        <v>99</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -7572,7 +7566,7 @@
         <v>50</v>
       </c>
       <c r="H15" s="5">
-        <v>99</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -7586,7 +7580,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -9523,7 +9517,7 @@
       </c>
       <c r="Z41" s="5"/>
     </row>
-    <row r="43" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="str">
         <f>Populations!$C$13</f>
         <v>Females 25-49</v>
@@ -9585,7 +9579,7 @@
       </c>
       <c r="Z43" s="5"/>
     </row>
-    <row r="44" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="str">
         <f>Populations!$C$13</f>
         <v>Females 25-49</v>
@@ -9647,7 +9641,7 @@
       </c>
       <c r="Z44" s="5"/>
     </row>
-    <row r="45" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="str">
         <f>Populations!$C$13</f>
         <v>Females 25-49</v>
@@ -9709,7 +9703,7 @@
       </c>
       <c r="Z45" s="5"/>
     </row>
-    <row r="47" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="str">
         <f>Populations!$C$14</f>
         <v>Males 50+</v>
@@ -9771,7 +9765,7 @@
       </c>
       <c r="Z47" s="5"/>
     </row>
-    <row r="48" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="str">
         <f>Populations!$C$14</f>
         <v>Males 50+</v>
@@ -9833,7 +9827,7 @@
       </c>
       <c r="Z48" s="5"/>
     </row>
-    <row r="49" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="str">
         <f>Populations!$C$14</f>
         <v>Males 50+</v>
@@ -9895,7 +9889,7 @@
       </c>
       <c r="Z49" s="5"/>
     </row>
-    <row r="51" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="str">
         <f>Populations!$C$15</f>
         <v>Females 50+</v>
@@ -9957,7 +9951,7 @@
       </c>
       <c r="Z51" s="5"/>
     </row>
-    <row r="52" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="str">
         <f>Populations!$C$15</f>
         <v>Females 50+</v>
@@ -10019,7 +10013,7 @@
       </c>
       <c r="Z52" s="5"/>
     </row>
-    <row r="53" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="str">
         <f>Populations!$C$15</f>
         <v>Females 50+</v>
@@ -10094,7 +10088,7 @@
       <selection activeCell="Z9" sqref="Z9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -11319,7 +11313,7 @@
       </c>
       <c r="Z41" s="7"/>
     </row>
-    <row r="43" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="str">
         <f>Populations!$C$13</f>
         <v>Females 25-49</v>
@@ -11359,7 +11353,7 @@
       </c>
       <c r="Z43" s="7"/>
     </row>
-    <row r="44" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="str">
         <f>Populations!$C$13</f>
         <v>Females 25-49</v>
@@ -11399,7 +11393,7 @@
       </c>
       <c r="Z44" s="7"/>
     </row>
-    <row r="45" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="str">
         <f>Populations!$C$13</f>
         <v>Females 25-49</v>
@@ -11439,7 +11433,7 @@
       </c>
       <c r="Z45" s="7"/>
     </row>
-    <row r="47" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="str">
         <f>Populations!$C$14</f>
         <v>Males 50+</v>
@@ -11479,7 +11473,7 @@
       </c>
       <c r="Z47" s="7"/>
     </row>
-    <row r="48" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="str">
         <f>Populations!$C$14</f>
         <v>Males 50+</v>
@@ -11519,7 +11513,7 @@
       </c>
       <c r="Z48" s="7"/>
     </row>
-    <row r="49" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="str">
         <f>Populations!$C$14</f>
         <v>Males 50+</v>
@@ -11559,7 +11553,7 @@
       </c>
       <c r="Z49" s="7"/>
     </row>
-    <row r="51" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="str">
         <f>Populations!$C$15</f>
         <v>Females 50+</v>
@@ -11599,7 +11593,7 @@
       </c>
       <c r="Z51" s="7"/>
     </row>
-    <row r="52" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="str">
         <f>Populations!$C$15</f>
         <v>Females 50+</v>
@@ -11639,7 +11633,7 @@
       </c>
       <c r="Z52" s="7"/>
     </row>
-    <row r="53" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="str">
         <f>Populations!$C$15</f>
         <v>Females 50+</v>
@@ -11690,7 +11684,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -12901,7 +12895,7 @@
         <v>3.8800000000000002E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>Females 0-9</v>
@@ -12934,7 +12928,7 @@
         <v>3.8800000000000002E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>Males 10-19</v>
@@ -12967,7 +12961,7 @@
         <v>3.8800000000000002E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>Females 10-19</v>
@@ -13000,7 +12994,7 @@
         <v>3.8800000000000002E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>Males 20-24</v>
@@ -13033,7 +13027,7 @@
         <v>3.8800000000000002E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>Females 20-24</v>
@@ -13066,7 +13060,7 @@
         <v>3.8800000000000002E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="str">
         <f>Populations!$C$12</f>
         <v>Males 25-49</v>
@@ -13099,7 +13093,7 @@
         <v>3.8800000000000002E-3</v>
       </c>
     </row>
-    <row r="49" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="str">
         <f>Populations!$C$13</f>
         <v>Females 25-49</v>
@@ -13132,7 +13126,7 @@
         <v>3.8800000000000002E-3</v>
       </c>
     </row>
-    <row r="50" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="str">
         <f>Populations!$C$14</f>
         <v>Males 50+</v>
@@ -13165,7 +13159,7 @@
         <v>3.8800000000000002E-3</v>
       </c>
     </row>
-    <row r="51" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="str">
         <f>Populations!$C$15</f>
         <v>Females 50+</v>
@@ -13207,11 +13201,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -14301,7 +14295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>Females 0-9</v>
@@ -14334,7 +14328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="str">
         <f>Populations!$C$8</f>
         <v>Males 10-19</v>
@@ -14367,7 +14361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>Females 10-19</v>
@@ -14400,7 +14394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="str">
         <f>Populations!$C$10</f>
         <v>Males 20-24</v>
@@ -14433,7 +14427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>Females 20-24</v>
@@ -14466,7 +14460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="str">
         <f>Populations!$C$12</f>
         <v>Males 25-49</v>
@@ -14499,7 +14493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="str">
         <f>Populations!$C$13</f>
         <v>Females 25-49</v>
@@ -14532,7 +14526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="str">
         <f>Populations!$C$14</f>
         <v>Males 50+</v>
@@ -14565,7 +14559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="str">
         <f>Populations!$C$15</f>
         <v>Females 50+</v>
@@ -14598,12 +14592,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C56" s="4">
         <v>2000</v>
       </c>
@@ -14671,7 +14665,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B57" s="4" t="s">
         <v>52</v>
       </c>
@@ -14713,12 +14707,12 @@
       </c>
       <c r="Y57" s="5"/>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C62" s="4">
         <v>2000</v>
       </c>
@@ -14786,7 +14780,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -14821,7 +14815,7 @@
       </c>
       <c r="Y63" s="9"/>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="str">
         <f>Populations!$C$7</f>
         <v>Females 0-9</v>
@@ -14854,7 +14848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="str">
         <f>Populations!$C$9</f>
         <v>Females 10-19</v>
@@ -14889,7 +14883,7 @@
       </c>
       <c r="Y65" s="9"/>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B66" s="4" t="str">
         <f>Populations!$C$11</f>
         <v>Females 20-24</v>
@@ -14924,7 +14918,7 @@
       </c>
       <c r="Y66" s="9"/>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B67" s="4" t="str">
         <f>Populations!$C$13</f>
         <v>Females 25-49</v>
@@ -14959,7 +14953,7 @@
       </c>
       <c r="Y67" s="9"/>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B68" s="4" t="str">
         <f>Populations!$C$15</f>
         <v>Females 50+</v>
@@ -14992,12 +14986,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C73" s="4">
         <v>2000</v>
       </c>
@@ -15065,7 +15059,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B74" s="4" t="s">
         <v>50</v>
       </c>
@@ -15114,7 +15108,7 @@
       <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -15885,12 +15879,12 @@
       </c>
       <c r="Y39" s="5"/>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C44" s="4">
         <v>2000</v>
       </c>
@@ -15958,7 +15952,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
         <v>50</v>
       </c>
@@ -15988,12 +15982,12 @@
       </c>
       <c r="Y45" s="8"/>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C50" s="4">
         <v>2000</v>
       </c>
@@ -16061,7 +16055,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
         <v>50</v>
       </c>
@@ -16091,12 +16085,12 @@
       </c>
       <c r="Y51" s="8"/>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C56" s="4">
         <v>2000</v>
       </c>
@@ -16164,7 +16158,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B57" s="4" t="s">
         <v>50</v>
       </c>
@@ -16194,12 +16188,12 @@
       </c>
       <c r="Y57" s="8"/>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C62" s="4">
         <v>2000</v>
       </c>
@@ -16267,7 +16261,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
         <v>50</v>
       </c>
@@ -16297,12 +16291,12 @@
       </c>
       <c r="Y63" s="8"/>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C68" s="4">
         <v>2000</v>
       </c>
@@ -16370,7 +16364,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B69" s="4" t="s">
         <v>50</v>
       </c>
@@ -16413,7 +16407,7 @@
       <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -17591,12 +17585,12 @@
       </c>
       <c r="Y39" s="8"/>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C44" s="4">
         <v>2000</v>
       </c>
@@ -17664,7 +17658,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
         <v>50</v>
       </c>
@@ -17698,12 +17692,12 @@
       </c>
       <c r="Y45" s="8"/>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C50" s="4">
         <v>2000</v>
       </c>
@@ -17771,7 +17765,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
         <v>52</v>
       </c>
@@ -17835,7 +17829,7 @@
   <sheetViews>
     <sheetView topLeftCell="A88" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">

</xml_diff>